<commit_message>
Added option to select taxa within Zoopsynther function, updated FRP crosswalk lifestages, and passed R CMD check.
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E083BF34-3CAF-4F20-A544-306C1BA4187F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3E438E-E184-41EC-9190-B20E56103838}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3917,9 +3917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8403,7 +8403,7 @@
         <v>384</v>
       </c>
       <c r="L75" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M75" s="31" t="s">
         <v>211</v>
@@ -8785,7 +8785,7 @@
       </c>
       <c r="K82" s="31"/>
       <c r="L82" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M82" s="31" t="s">
         <v>94</v>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="K86" s="31"/>
       <c r="L86" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M86" s="31" t="s">
         <v>231</v>
@@ -9407,7 +9407,7 @@
       </c>
       <c r="K95" s="31"/>
       <c r="L95" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M95" s="31" t="s">
         <v>251</v>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="K114" s="31"/>
       <c r="L114" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M114" s="31" t="s">
         <v>278</v>
@@ -10485,7 +10485,7 @@
       </c>
       <c r="K117" s="31"/>
       <c r="L117" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M117" s="31" t="s">
         <v>330</v>
@@ -10681,7 +10681,7 @@
       </c>
       <c r="K121" s="31"/>
       <c r="L121" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M121" s="31" t="s">
         <v>293</v>
@@ -11203,7 +11203,7 @@
       </c>
       <c r="K132" s="31"/>
       <c r="L132" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M132" s="31" t="s">
         <v>300</v>
@@ -11441,7 +11441,7 @@
       </c>
       <c r="K137" s="31"/>
       <c r="L137" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M137" s="31" t="s">
         <v>310</v>
@@ -11781,7 +11781,7 @@
       </c>
       <c r="K144" s="31"/>
       <c r="L144" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M144" s="31" t="s">
         <v>321</v>
@@ -13525,7 +13525,7 @@
       </c>
       <c r="K179" s="31"/>
       <c r="L179" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M179" s="33" t="s">
         <v>504</v>
@@ -13575,7 +13575,7 @@
       </c>
       <c r="K180" s="31"/>
       <c r="L180" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M180" s="36" t="s">
         <v>308</v>
@@ -13619,7 +13619,7 @@
       </c>
       <c r="K181" s="31"/>
       <c r="L181" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M181" s="33" t="s">
         <v>505</v>
@@ -18895,7 +18895,7 @@
       </c>
       <c r="K290" s="31"/>
       <c r="L290" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M290" s="33" t="s">
         <v>102</v>
@@ -18991,7 +18991,7 @@
       </c>
       <c r="K292" s="31"/>
       <c r="L292" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M292" s="33" t="s">
         <v>262</v>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="K293" s="31"/>
       <c r="L293" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M293" s="33" t="s">
         <v>688</v>
@@ -19083,7 +19083,7 @@
       </c>
       <c r="K294" s="31"/>
       <c r="L294" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M294" s="33" t="s">
         <v>262</v>
@@ -19125,7 +19125,7 @@
       </c>
       <c r="K295" s="31"/>
       <c r="L295" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M295" s="33" t="s">
         <v>691</v>
@@ -19175,7 +19175,7 @@
       </c>
       <c r="K296" s="31"/>
       <c r="L296" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M296" s="33" t="s">
         <v>696</v>
@@ -19659,7 +19659,7 @@
       </c>
       <c r="K306" s="31"/>
       <c r="L306" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M306" s="33" t="s">
         <v>721</v>
@@ -19943,7 +19943,7 @@
       </c>
       <c r="K312" s="31"/>
       <c r="L312" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M312" s="33" t="s">
         <v>732</v>
@@ -19993,7 +19993,7 @@
       </c>
       <c r="K313" s="31"/>
       <c r="L313" s="31" t="s">
-        <v>207</v>
+        <v>787</v>
       </c>
       <c r="M313" s="33" t="s">
         <v>733</v>

</xml_diff>

<commit_message>
Updated data to fit revised crosswalk, fixed some `dtplyr` issues in zoop downloader.
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3E438E-E184-41EC-9190-B20E56103838}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25338742-230F-4F72-99F1-E938B03EC087}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3918,8 +3918,8 @@
   <dimension ref="A1:AB318"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J108" sqref="J108"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8403,7 +8403,7 @@
         <v>384</v>
       </c>
       <c r="L75" s="31" t="s">
-        <v>787</v>
+        <v>207</v>
       </c>
       <c r="M75" s="31" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Fixed typo in crosswalk
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D9C58-8BAC-4A4A-9680-CAC68C909B32}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A36D9F-DE51-4C08-B19D-50C99E10CB0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="-2604" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCD" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="789">
   <si>
     <t>ACARTELA</t>
   </si>
@@ -2473,6 +2473,9 @@
   </si>
   <si>
     <t>Pupa</t>
+  </si>
+  <si>
+    <t>Hydrachnidia</t>
   </si>
 </sst>
 </file>
@@ -3917,9 +3920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K296" sqref="K296"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M124" sqref="M124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10964,7 +10967,7 @@
         <v>207</v>
       </c>
       <c r="M127" s="31" t="s">
-        <v>736</v>
+        <v>788</v>
       </c>
       <c r="N127" s="31" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Added more flexibility to `zoop_downloader` so the package will not break when dates are changed in the source dataset filenames and changed Summer Townet acronym from TNS to STN.
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A36D9F-DE51-4C08-B19D-50C99E10CB0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A1C648-4586-4891-BB1C-425B89B3493D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="-2604" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCD" sheetId="4" r:id="rId1"/>
@@ -2418,12 +2418,6 @@
     <t>EMP_Macro</t>
   </si>
   <si>
-    <t>TNS_Meso</t>
-  </si>
-  <si>
-    <t>TNS_Macro</t>
-  </si>
-  <si>
     <t>FMWT_Meso</t>
   </si>
   <si>
@@ -2476,6 +2470,12 @@
   </si>
   <si>
     <t>Hydrachnidia</t>
+  </si>
+  <si>
+    <t>STN_Meso</t>
+  </si>
+  <si>
+    <t>STN_Macro</t>
   </si>
 </sst>
 </file>
@@ -3920,9 +3920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M124" sqref="M124"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3962,25 +3962,25 @@
         <v>768</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>788</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>769</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>770</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>771</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>772</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>773</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>774</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>775</v>
       </c>
       <c r="K1" s="31" t="s">
         <v>486</v>
@@ -5832,7 +5832,7 @@
         <v>384</v>
       </c>
       <c r="L31" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M31" s="31" t="s">
         <v>133</v>
@@ -6942,7 +6942,7 @@
         <v>375</v>
       </c>
       <c r="L50" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M50" s="31" t="s">
         <v>101</v>
@@ -6994,7 +6994,7 @@
       </c>
       <c r="K51" s="31"/>
       <c r="L51" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M51" s="31" t="s">
         <v>116</v>
@@ -7050,7 +7050,7 @@
       <c r="J52" s="31"/>
       <c r="K52" s="31"/>
       <c r="L52" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M52" s="31" t="s">
         <v>6</v>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="K53" s="31"/>
       <c r="L53" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M53" s="31" t="s">
         <v>101</v>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="K54" s="31"/>
       <c r="L54" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M54" s="31" t="s">
         <v>114</v>
@@ -7228,7 +7228,7 @@
       <c r="J55" s="31"/>
       <c r="K55" s="31"/>
       <c r="L55" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M55" s="31" t="s">
         <v>117</v>
@@ -7290,7 +7290,7 @@
       </c>
       <c r="K56" s="31"/>
       <c r="L56" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M56" s="31" t="s">
         <v>14</v>
@@ -7346,7 +7346,7 @@
         <v>403</v>
       </c>
       <c r="L57" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M57" s="31" t="s">
         <v>93</v>
@@ -7386,7 +7386,7 @@
         <v>404</v>
       </c>
       <c r="L58" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M58" s="31" t="s">
         <v>136</v>
@@ -8288,7 +8288,7 @@
         <v>388</v>
       </c>
       <c r="L73" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M73" s="31" t="s">
         <v>213</v>
@@ -8346,7 +8346,7 @@
       </c>
       <c r="K74" s="31"/>
       <c r="L74" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M74" s="31" t="s">
         <v>144</v>
@@ -8562,7 +8562,7 @@
         <v>381</v>
       </c>
       <c r="L78" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M78" s="31" t="s">
         <v>95</v>
@@ -8618,7 +8618,7 @@
         <v>385</v>
       </c>
       <c r="L79" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M79" s="31" t="s">
         <v>94</v>
@@ -8788,7 +8788,7 @@
       </c>
       <c r="K82" s="31"/>
       <c r="L82" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M82" s="31" t="s">
         <v>94</v>
@@ -8974,7 +8974,7 @@
       </c>
       <c r="K86" s="31"/>
       <c r="L86" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M86" s="31" t="s">
         <v>230</v>
@@ -9114,7 +9114,7 @@
       </c>
       <c r="K89" s="31"/>
       <c r="L89" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M89" s="31" t="s">
         <v>236</v>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="K93" s="31"/>
       <c r="L93" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M93" s="31" t="s">
         <v>247</v>
@@ -9410,7 +9410,7 @@
       </c>
       <c r="K95" s="31"/>
       <c r="L95" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M95" s="31" t="s">
         <v>250</v>
@@ -9638,7 +9638,7 @@
       </c>
       <c r="K100" s="31"/>
       <c r="L100" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M100" s="31" t="s">
         <v>246</v>
@@ -9952,7 +9952,7 @@
       </c>
       <c r="K106" s="31"/>
       <c r="L106" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M106" s="31" t="s">
         <v>268</v>
@@ -10050,7 +10050,7 @@
       </c>
       <c r="K108" s="31"/>
       <c r="L108" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M108" s="31" t="s">
         <v>270</v>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="K112" s="31"/>
       <c r="L112" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M112" s="31" t="s">
         <v>273</v>
@@ -10352,7 +10352,7 @@
       </c>
       <c r="K114" s="31"/>
       <c r="L114" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M114" s="31" t="s">
         <v>277</v>
@@ -10396,7 +10396,7 @@
       </c>
       <c r="K115" s="31"/>
       <c r="L115" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M115" s="31" t="s">
         <v>278</v>
@@ -10442,7 +10442,7 @@
       </c>
       <c r="K116" s="31"/>
       <c r="L116" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M116" s="31" t="s">
         <v>199</v>
@@ -10488,7 +10488,7 @@
       </c>
       <c r="K117" s="31"/>
       <c r="L117" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M117" s="31" t="s">
         <v>328</v>
@@ -10684,7 +10684,7 @@
       </c>
       <c r="K121" s="31"/>
       <c r="L121" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M121" s="31" t="s">
         <v>292</v>
@@ -10872,7 +10872,7 @@
       </c>
       <c r="K125" s="31"/>
       <c r="L125" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M125" s="31" t="s">
         <v>199</v>
@@ -10911,14 +10911,14 @@
       <c r="G126" s="38"/>
       <c r="H126" s="31"/>
       <c r="I126" s="31" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="J126" s="31" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="K126" s="31"/>
       <c r="L126" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M126" s="31" t="s">
         <v>199</v>
@@ -10967,7 +10967,7 @@
         <v>207</v>
       </c>
       <c r="M127" s="31" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="N127" s="31" t="s">
         <v>84</v>
@@ -11206,7 +11206,7 @@
       </c>
       <c r="K132" s="31"/>
       <c r="L132" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M132" s="31" t="s">
         <v>298</v>
@@ -11444,7 +11444,7 @@
       </c>
       <c r="K137" s="31"/>
       <c r="L137" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M137" s="31" t="s">
         <v>308</v>
@@ -11784,7 +11784,7 @@
       </c>
       <c r="K144" s="31"/>
       <c r="L144" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M144" s="31" t="s">
         <v>319</v>
@@ -13528,7 +13528,7 @@
       </c>
       <c r="K179" s="31"/>
       <c r="L179" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M179" s="33" t="s">
         <v>502</v>
@@ -13578,7 +13578,7 @@
       </c>
       <c r="K180" s="31"/>
       <c r="L180" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M180" s="36" t="s">
         <v>306</v>
@@ -13622,7 +13622,7 @@
       </c>
       <c r="K181" s="31"/>
       <c r="L181" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M181" s="33" t="s">
         <v>503</v>
@@ -13912,7 +13912,7 @@
       </c>
       <c r="K187" s="31"/>
       <c r="L187" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M187" s="33" t="s">
         <v>741</v>
@@ -14054,7 +14054,7 @@
       </c>
       <c r="K190" s="31"/>
       <c r="L190" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M190" s="33" t="s">
         <v>516</v>
@@ -14342,7 +14342,7 @@
       </c>
       <c r="K196" s="31"/>
       <c r="L196" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M196" s="33" t="s">
         <v>522</v>
@@ -14390,7 +14390,7 @@
       </c>
       <c r="K197" s="31"/>
       <c r="L197" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M197" s="33" t="s">
         <v>525</v>
@@ -14438,7 +14438,7 @@
       </c>
       <c r="K198" s="31"/>
       <c r="L198" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M198" s="33" t="s">
         <v>519</v>
@@ -14584,7 +14584,7 @@
       </c>
       <c r="K201" s="31"/>
       <c r="L201" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M201" s="33" t="s">
         <v>532</v>
@@ -14632,7 +14632,7 @@
       </c>
       <c r="K202" s="31"/>
       <c r="L202" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M202" s="33" t="s">
         <v>534</v>
@@ -14920,7 +14920,7 @@
       </c>
       <c r="K208" s="31"/>
       <c r="L208" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M208" s="33" t="s">
         <v>537</v>
@@ -15062,7 +15062,7 @@
       </c>
       <c r="K211" s="31"/>
       <c r="L211" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M211" s="33" t="s">
         <v>549</v>
@@ -15110,7 +15110,7 @@
       </c>
       <c r="K212" s="31"/>
       <c r="L212" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M212" s="33" t="s">
         <v>199</v>
@@ -15156,7 +15156,7 @@
       </c>
       <c r="K213" s="31"/>
       <c r="L213" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M213" s="33" t="s">
         <v>199</v>
@@ -15202,7 +15202,7 @@
       </c>
       <c r="K214" s="31"/>
       <c r="L214" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M214" s="33" t="s">
         <v>199</v>
@@ -15248,7 +15248,7 @@
       </c>
       <c r="K215" s="31"/>
       <c r="L215" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M215" s="33" t="s">
         <v>554</v>
@@ -15296,7 +15296,7 @@
       </c>
       <c r="K216" s="31"/>
       <c r="L216" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M216" s="33" t="s">
         <v>555</v>
@@ -15344,7 +15344,7 @@
       </c>
       <c r="K217" s="31"/>
       <c r="L217" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M217" s="33" t="s">
         <v>199</v>
@@ -15390,7 +15390,7 @@
       </c>
       <c r="K218" s="31"/>
       <c r="L218" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M218" s="33" t="s">
         <v>558</v>
@@ -15438,7 +15438,7 @@
       </c>
       <c r="K219" s="31"/>
       <c r="L219" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M219" s="33" t="s">
         <v>560</v>
@@ -15486,7 +15486,7 @@
       </c>
       <c r="K220" s="31"/>
       <c r="L220" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M220" s="33" t="s">
         <v>562</v>
@@ -15534,7 +15534,7 @@
       </c>
       <c r="K221" s="31"/>
       <c r="L221" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M221" s="33" t="s">
         <v>564</v>
@@ -15582,7 +15582,7 @@
       </c>
       <c r="K222" s="31"/>
       <c r="L222" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M222" s="33" t="s">
         <v>566</v>
@@ -15630,7 +15630,7 @@
       </c>
       <c r="K223" s="31"/>
       <c r="L223" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M223" s="33" t="s">
         <v>568</v>
@@ -15678,7 +15678,7 @@
       </c>
       <c r="K224" s="31"/>
       <c r="L224" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M224" s="33" t="s">
         <v>570</v>
@@ -15726,7 +15726,7 @@
       </c>
       <c r="K225" s="31"/>
       <c r="L225" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M225" s="33" t="s">
         <v>571</v>
@@ -15774,7 +15774,7 @@
       </c>
       <c r="K226" s="31"/>
       <c r="L226" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M226" s="33" t="s">
         <v>572</v>
@@ -15822,7 +15822,7 @@
       </c>
       <c r="K227" s="31"/>
       <c r="L227" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M227" s="33" t="s">
         <v>278</v>
@@ -15868,7 +15868,7 @@
       </c>
       <c r="K228" s="31"/>
       <c r="L228" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M228" s="33" t="s">
         <v>575</v>
@@ -15916,7 +15916,7 @@
       </c>
       <c r="K229" s="31"/>
       <c r="L229" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M229" s="31" t="s">
         <v>580</v>
@@ -16538,7 +16538,7 @@
       </c>
       <c r="K242" s="31"/>
       <c r="L242" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M242" s="33" t="s">
         <v>224</v>
@@ -16632,7 +16632,7 @@
       </c>
       <c r="K244" s="31"/>
       <c r="L244" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M244" s="33" t="s">
         <v>597</v>
@@ -16724,7 +16724,7 @@
       </c>
       <c r="K246" s="31"/>
       <c r="L246" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M246" s="33" t="s">
         <v>597</v>
@@ -16770,7 +16770,7 @@
       </c>
       <c r="K247" s="31"/>
       <c r="L247" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M247" s="33" t="s">
         <v>602</v>
@@ -16818,7 +16818,7 @@
       </c>
       <c r="K248" s="31"/>
       <c r="L248" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M248" s="33" t="s">
         <v>745</v>
@@ -16912,7 +16912,7 @@
       </c>
       <c r="K250" s="31"/>
       <c r="L250" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M250" s="33" t="s">
         <v>606</v>
@@ -16960,7 +16960,7 @@
       </c>
       <c r="K251" s="31"/>
       <c r="L251" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M251" s="33" t="s">
         <v>267</v>
@@ -17006,7 +17006,7 @@
       </c>
       <c r="K252" s="31"/>
       <c r="L252" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M252" s="33" t="s">
         <v>608</v>
@@ -17146,7 +17146,7 @@
       </c>
       <c r="K255" s="31"/>
       <c r="L255" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M255" s="33" t="s">
         <v>611</v>
@@ -17192,7 +17192,7 @@
       </c>
       <c r="K256" s="31"/>
       <c r="L256" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M256" s="33" t="s">
         <v>246</v>
@@ -17286,7 +17286,7 @@
       </c>
       <c r="K258" s="31"/>
       <c r="L258" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M258" s="33" t="s">
         <v>746</v>
@@ -17380,7 +17380,7 @@
       </c>
       <c r="K260" s="31"/>
       <c r="L260" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M260" s="33" t="s">
         <v>247</v>
@@ -17428,7 +17428,7 @@
       </c>
       <c r="K261" s="31"/>
       <c r="L261" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M261" s="33" t="s">
         <v>94</v>
@@ -17722,7 +17722,7 @@
       </c>
       <c r="K267" s="31"/>
       <c r="L267" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M267" s="33" t="s">
         <v>144</v>
@@ -18823,7 +18823,7 @@
       <c r="A289" s="34"/>
       <c r="B289" s="34"/>
       <c r="C289" s="34" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D289" s="31"/>
       <c r="E289" s="31" t="s">
@@ -18898,7 +18898,7 @@
       </c>
       <c r="K290" s="31"/>
       <c r="L290" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M290" s="33" t="s">
         <v>102</v>
@@ -18994,7 +18994,7 @@
       </c>
       <c r="K292" s="31"/>
       <c r="L292" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M292" s="33" t="s">
         <v>261</v>
@@ -19036,7 +19036,7 @@
       </c>
       <c r="K293" s="31"/>
       <c r="L293" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M293" s="33" t="s">
         <v>686</v>
@@ -19086,7 +19086,7 @@
       </c>
       <c r="K294" s="31"/>
       <c r="L294" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M294" s="33" t="s">
         <v>261</v>
@@ -19128,7 +19128,7 @@
       </c>
       <c r="K295" s="31"/>
       <c r="L295" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M295" s="33" t="s">
         <v>689</v>
@@ -19178,7 +19178,7 @@
       </c>
       <c r="K296" s="31"/>
       <c r="L296" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M296" s="33" t="s">
         <v>694</v>
@@ -19413,10 +19413,10 @@
       <c r="G301" s="31"/>
       <c r="H301" s="31"/>
       <c r="I301" s="33" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="J301" s="33" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="K301" s="31"/>
       <c r="L301" s="31" t="s">
@@ -19662,7 +19662,7 @@
       </c>
       <c r="K306" s="31"/>
       <c r="L306" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M306" s="33" t="s">
         <v>719</v>
@@ -19946,7 +19946,7 @@
       </c>
       <c r="K312" s="31"/>
       <c r="L312" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M312" s="33" t="s">
         <v>730</v>
@@ -19996,7 +19996,7 @@
       </c>
       <c r="K313" s="31"/>
       <c r="L313" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M313" s="33" t="s">
         <v>731</v>
@@ -20038,7 +20038,7 @@
       </c>
       <c r="K314" s="31"/>
       <c r="L314" s="31" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M314" s="33" t="s">
         <v>735</v>
@@ -20061,38 +20061,38 @@
     </row>
     <row r="315" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I315" s="37" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="J315" s="37" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="L315" s="37" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="M315" s="37" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="316" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I316" s="39" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="J316" s="39" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="L316" s="37" t="s">
+        <v>777</v>
+      </c>
+      <c r="M316" s="37" t="s">
         <v>779</v>
-      </c>
-      <c r="M316" s="37" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="317" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I317" s="37" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="J317" s="37" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="L317" s="31" t="s">
         <v>207</v>
@@ -20118,13 +20118,13 @@
     </row>
     <row r="318" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I318" s="37" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="J318" s="37" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="L318" s="37" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="M318" s="37" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
Moved EMP source to EDI
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A1C648-4586-4891-BB1C-425B89B3493D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44073987-105A-4959-BA04-1A15DD496582}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="-2604" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCD" sheetId="4" r:id="rId1"/>
@@ -2367,27 +2367,6 @@
     <t>limnicola</t>
   </si>
   <si>
-    <t>A_ aspera</t>
-  </si>
-  <si>
-    <t>A_ hwanhaiensis</t>
-  </si>
-  <si>
-    <t>A_ macropsis</t>
-  </si>
-  <si>
-    <t>D_ holmquistae</t>
-  </si>
-  <si>
-    <t>N_ kadiakensis</t>
-  </si>
-  <si>
-    <t>N_ mercedis</t>
-  </si>
-  <si>
-    <t>Unidentified mysid</t>
-  </si>
-  <si>
     <t>Unidentified Mysid</t>
   </si>
   <si>
@@ -2433,9 +2412,6 @@
     <t>FRP_Macro</t>
   </si>
   <si>
-    <t>H_ longirostris</t>
-  </si>
-  <si>
     <t>Diptera pupae</t>
   </si>
   <si>
@@ -2476,6 +2452,30 @@
   </si>
   <si>
     <t>STN_Macro</t>
+  </si>
+  <si>
+    <t>A_aspera</t>
+  </si>
+  <si>
+    <t>N_mercedis</t>
+  </si>
+  <si>
+    <t>N_kadiakensis</t>
+  </si>
+  <si>
+    <t>A_hwanhaiensis</t>
+  </si>
+  <si>
+    <t>A_macropsis</t>
+  </si>
+  <si>
+    <t>D_holmquistae</t>
+  </si>
+  <si>
+    <t>Unidentified_mysid</t>
+  </si>
+  <si>
+    <t>H_longirostris</t>
   </si>
 </sst>
 </file>
@@ -3921,8 +3921,8 @@
   <dimension ref="A1:AB318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G135" sqref="G135"/>
+      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C290" sqref="C290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3953,34 +3953,34 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
+        <v>759</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>760</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>761</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>779</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>780</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>762</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>763</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>764</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>765</v>
+      </c>
+      <c r="J1" s="31" t="s">
         <v>766</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>767</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>768</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>787</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>788</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>769</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>770</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>771</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>772</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>773</v>
       </c>
       <c r="K1" s="31" t="s">
         <v>486</v>
@@ -5832,7 +5832,7 @@
         <v>384</v>
       </c>
       <c r="L31" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M31" s="31" t="s">
         <v>133</v>
@@ -6942,7 +6942,7 @@
         <v>375</v>
       </c>
       <c r="L50" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M50" s="31" t="s">
         <v>101</v>
@@ -6994,7 +6994,7 @@
       </c>
       <c r="K51" s="31"/>
       <c r="L51" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M51" s="31" t="s">
         <v>116</v>
@@ -7050,7 +7050,7 @@
       <c r="J52" s="31"/>
       <c r="K52" s="31"/>
       <c r="L52" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M52" s="31" t="s">
         <v>6</v>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="K53" s="31"/>
       <c r="L53" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M53" s="31" t="s">
         <v>101</v>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="K54" s="31"/>
       <c r="L54" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M54" s="31" t="s">
         <v>114</v>
@@ -7228,7 +7228,7 @@
       <c r="J55" s="31"/>
       <c r="K55" s="31"/>
       <c r="L55" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M55" s="31" t="s">
         <v>117</v>
@@ -7290,7 +7290,7 @@
       </c>
       <c r="K56" s="31"/>
       <c r="L56" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M56" s="31" t="s">
         <v>14</v>
@@ -7346,7 +7346,7 @@
         <v>403</v>
       </c>
       <c r="L57" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M57" s="31" t="s">
         <v>93</v>
@@ -7386,7 +7386,7 @@
         <v>404</v>
       </c>
       <c r="L58" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M58" s="31" t="s">
         <v>136</v>
@@ -8288,7 +8288,7 @@
         <v>388</v>
       </c>
       <c r="L73" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M73" s="31" t="s">
         <v>213</v>
@@ -8346,7 +8346,7 @@
       </c>
       <c r="K74" s="31"/>
       <c r="L74" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M74" s="31" t="s">
         <v>144</v>
@@ -8562,7 +8562,7 @@
         <v>381</v>
       </c>
       <c r="L78" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M78" s="31" t="s">
         <v>95</v>
@@ -8618,7 +8618,7 @@
         <v>385</v>
       </c>
       <c r="L79" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M79" s="31" t="s">
         <v>94</v>
@@ -8653,7 +8653,7 @@
       <c r="A80" s="34"/>
       <c r="B80" s="34"/>
       <c r="C80" s="34" t="s">
-        <v>752</v>
+        <v>781</v>
       </c>
       <c r="D80" s="31"/>
       <c r="E80" s="31" t="s">
@@ -8719,11 +8719,11 @@
       <c r="C81" s="31"/>
       <c r="D81" s="38"/>
       <c r="E81" s="38" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="F81" s="38"/>
       <c r="G81" s="38" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="H81" s="31" t="s">
         <v>221</v>
@@ -8788,7 +8788,7 @@
       </c>
       <c r="K82" s="31"/>
       <c r="L82" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M82" s="31" t="s">
         <v>94</v>
@@ -8974,7 +8974,7 @@
       </c>
       <c r="K86" s="31"/>
       <c r="L86" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M86" s="31" t="s">
         <v>230</v>
@@ -9114,7 +9114,7 @@
       </c>
       <c r="K89" s="31"/>
       <c r="L89" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M89" s="31" t="s">
         <v>236</v>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="K93" s="31"/>
       <c r="L93" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M93" s="31" t="s">
         <v>247</v>
@@ -9410,7 +9410,7 @@
       </c>
       <c r="K95" s="31"/>
       <c r="L95" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M95" s="31" t="s">
         <v>250</v>
@@ -9638,7 +9638,7 @@
       </c>
       <c r="K100" s="31"/>
       <c r="L100" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M100" s="31" t="s">
         <v>246</v>
@@ -9775,11 +9775,11 @@
       <c r="C103" s="31"/>
       <c r="D103" s="38"/>
       <c r="E103" s="38" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="F103" s="38"/>
       <c r="G103" s="38" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="H103" s="31"/>
       <c r="I103" s="31" t="s">
@@ -9879,7 +9879,7 @@
       <c r="A105" s="34"/>
       <c r="B105" s="34"/>
       <c r="C105" s="34" t="s">
-        <v>757</v>
+        <v>782</v>
       </c>
       <c r="D105" s="38"/>
       <c r="E105" s="38" t="s">
@@ -9952,7 +9952,7 @@
       </c>
       <c r="K106" s="31"/>
       <c r="L106" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M106" s="31" t="s">
         <v>268</v>
@@ -10050,7 +10050,7 @@
       </c>
       <c r="K108" s="31"/>
       <c r="L108" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M108" s="31" t="s">
         <v>270</v>
@@ -10181,7 +10181,7 @@
       <c r="A111" s="34"/>
       <c r="B111" s="34"/>
       <c r="C111" s="34" t="s">
-        <v>756</v>
+        <v>783</v>
       </c>
       <c r="D111" s="38"/>
       <c r="E111" s="38" t="s">
@@ -10254,7 +10254,7 @@
       </c>
       <c r="K112" s="31"/>
       <c r="L112" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M112" s="31" t="s">
         <v>273</v>
@@ -10352,7 +10352,7 @@
       </c>
       <c r="K114" s="31"/>
       <c r="L114" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M114" s="31" t="s">
         <v>277</v>
@@ -10396,7 +10396,7 @@
       </c>
       <c r="K115" s="31"/>
       <c r="L115" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M115" s="31" t="s">
         <v>278</v>
@@ -10442,7 +10442,7 @@
       </c>
       <c r="K116" s="31"/>
       <c r="L116" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M116" s="31" t="s">
         <v>199</v>
@@ -10488,7 +10488,7 @@
       </c>
       <c r="K117" s="31"/>
       <c r="L117" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M117" s="31" t="s">
         <v>328</v>
@@ -10684,7 +10684,7 @@
       </c>
       <c r="K121" s="31"/>
       <c r="L121" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M121" s="31" t="s">
         <v>292</v>
@@ -10717,11 +10717,11 @@
       <c r="C122" s="31"/>
       <c r="D122" s="38"/>
       <c r="E122" s="38" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="F122" s="38"/>
       <c r="G122" s="38" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="H122" s="31"/>
       <c r="I122" s="31" t="s">
@@ -10811,11 +10811,11 @@
       <c r="C124" s="31"/>
       <c r="D124" s="38"/>
       <c r="E124" s="38" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="F124" s="38"/>
       <c r="G124" s="38" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="H124" s="31"/>
       <c r="I124" s="31" t="s">
@@ -10872,7 +10872,7 @@
       </c>
       <c r="K125" s="31"/>
       <c r="L125" s="31" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="M125" s="31" t="s">
         <v>199</v>
@@ -10911,14 +10911,14 @@
       <c r="G126" s="38"/>
       <c r="H126" s="31"/>
       <c r="I126" s="31" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="J126" s="31" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="K126" s="31"/>
       <c r="L126" s="31" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="M126" s="31" t="s">
         <v>199</v>
@@ -10967,7 +10967,7 @@
         <v>207</v>
       </c>
       <c r="M127" s="31" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="N127" s="31" t="s">
         <v>84</v>
@@ -11206,7 +11206,7 @@
       </c>
       <c r="K132" s="31"/>
       <c r="L132" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M132" s="31" t="s">
         <v>298</v>
@@ -11444,7 +11444,7 @@
       </c>
       <c r="K137" s="31"/>
       <c r="L137" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M137" s="31" t="s">
         <v>308</v>
@@ -11481,11 +11481,11 @@
       <c r="C138" s="31"/>
       <c r="D138" s="38"/>
       <c r="E138" s="38" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="F138" s="38"/>
       <c r="G138" s="38" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="H138" s="31"/>
       <c r="I138" s="31" t="s">
@@ -11784,7 +11784,7 @@
       </c>
       <c r="K144" s="31"/>
       <c r="L144" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M144" s="31" t="s">
         <v>319</v>
@@ -13528,7 +13528,7 @@
       </c>
       <c r="K179" s="31"/>
       <c r="L179" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M179" s="33" t="s">
         <v>502</v>
@@ -13578,7 +13578,7 @@
       </c>
       <c r="K180" s="31"/>
       <c r="L180" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M180" s="36" t="s">
         <v>306</v>
@@ -13622,7 +13622,7 @@
       </c>
       <c r="K181" s="31"/>
       <c r="L181" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M181" s="33" t="s">
         <v>503</v>
@@ -13912,7 +13912,7 @@
       </c>
       <c r="K187" s="31"/>
       <c r="L187" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M187" s="33" t="s">
         <v>741</v>
@@ -14054,7 +14054,7 @@
       </c>
       <c r="K190" s="31"/>
       <c r="L190" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M190" s="33" t="s">
         <v>516</v>
@@ -14342,7 +14342,7 @@
       </c>
       <c r="K196" s="31"/>
       <c r="L196" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M196" s="33" t="s">
         <v>522</v>
@@ -14390,7 +14390,7 @@
       </c>
       <c r="K197" s="31"/>
       <c r="L197" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M197" s="33" t="s">
         <v>525</v>
@@ -14438,7 +14438,7 @@
       </c>
       <c r="K198" s="31"/>
       <c r="L198" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M198" s="33" t="s">
         <v>519</v>
@@ -14584,7 +14584,7 @@
       </c>
       <c r="K201" s="31"/>
       <c r="L201" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M201" s="33" t="s">
         <v>532</v>
@@ -14632,7 +14632,7 @@
       </c>
       <c r="K202" s="31"/>
       <c r="L202" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M202" s="33" t="s">
         <v>534</v>
@@ -14920,7 +14920,7 @@
       </c>
       <c r="K208" s="31"/>
       <c r="L208" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M208" s="33" t="s">
         <v>537</v>
@@ -15062,7 +15062,7 @@
       </c>
       <c r="K211" s="31"/>
       <c r="L211" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M211" s="33" t="s">
         <v>549</v>
@@ -15110,7 +15110,7 @@
       </c>
       <c r="K212" s="31"/>
       <c r="L212" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M212" s="33" t="s">
         <v>199</v>
@@ -15156,7 +15156,7 @@
       </c>
       <c r="K213" s="31"/>
       <c r="L213" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M213" s="33" t="s">
         <v>199</v>
@@ -15202,7 +15202,7 @@
       </c>
       <c r="K214" s="31"/>
       <c r="L214" s="31" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="M214" s="33" t="s">
         <v>199</v>
@@ -15248,7 +15248,7 @@
       </c>
       <c r="K215" s="31"/>
       <c r="L215" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M215" s="33" t="s">
         <v>554</v>
@@ -15296,7 +15296,7 @@
       </c>
       <c r="K216" s="31"/>
       <c r="L216" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M216" s="33" t="s">
         <v>555</v>
@@ -15344,7 +15344,7 @@
       </c>
       <c r="K217" s="31"/>
       <c r="L217" s="31" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="M217" s="33" t="s">
         <v>199</v>
@@ -15390,7 +15390,7 @@
       </c>
       <c r="K218" s="31"/>
       <c r="L218" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M218" s="33" t="s">
         <v>558</v>
@@ -15438,7 +15438,7 @@
       </c>
       <c r="K219" s="31"/>
       <c r="L219" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M219" s="33" t="s">
         <v>560</v>
@@ -15486,7 +15486,7 @@
       </c>
       <c r="K220" s="31"/>
       <c r="L220" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M220" s="33" t="s">
         <v>562</v>
@@ -15534,7 +15534,7 @@
       </c>
       <c r="K221" s="31"/>
       <c r="L221" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M221" s="33" t="s">
         <v>564</v>
@@ -15582,7 +15582,7 @@
       </c>
       <c r="K222" s="31"/>
       <c r="L222" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M222" s="33" t="s">
         <v>566</v>
@@ -15630,7 +15630,7 @@
       </c>
       <c r="K223" s="31"/>
       <c r="L223" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M223" s="33" t="s">
         <v>568</v>
@@ -15678,7 +15678,7 @@
       </c>
       <c r="K224" s="31"/>
       <c r="L224" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M224" s="33" t="s">
         <v>570</v>
@@ -15726,7 +15726,7 @@
       </c>
       <c r="K225" s="31"/>
       <c r="L225" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M225" s="33" t="s">
         <v>571</v>
@@ -15774,7 +15774,7 @@
       </c>
       <c r="K226" s="31"/>
       <c r="L226" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M226" s="33" t="s">
         <v>572</v>
@@ -15822,7 +15822,7 @@
       </c>
       <c r="K227" s="31"/>
       <c r="L227" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M227" s="33" t="s">
         <v>278</v>
@@ -15868,7 +15868,7 @@
       </c>
       <c r="K228" s="31"/>
       <c r="L228" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M228" s="33" t="s">
         <v>575</v>
@@ -15916,7 +15916,7 @@
       </c>
       <c r="K229" s="31"/>
       <c r="L229" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M229" s="31" t="s">
         <v>580</v>
@@ -16538,7 +16538,7 @@
       </c>
       <c r="K242" s="31"/>
       <c r="L242" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M242" s="33" t="s">
         <v>224</v>
@@ -16632,7 +16632,7 @@
       </c>
       <c r="K244" s="31"/>
       <c r="L244" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M244" s="33" t="s">
         <v>597</v>
@@ -16724,7 +16724,7 @@
       </c>
       <c r="K246" s="31"/>
       <c r="L246" s="31" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="M246" s="33" t="s">
         <v>597</v>
@@ -16770,7 +16770,7 @@
       </c>
       <c r="K247" s="31"/>
       <c r="L247" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M247" s="33" t="s">
         <v>602</v>
@@ -16818,7 +16818,7 @@
       </c>
       <c r="K248" s="31"/>
       <c r="L248" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M248" s="33" t="s">
         <v>745</v>
@@ -16912,7 +16912,7 @@
       </c>
       <c r="K250" s="31"/>
       <c r="L250" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M250" s="33" t="s">
         <v>606</v>
@@ -16960,7 +16960,7 @@
       </c>
       <c r="K251" s="31"/>
       <c r="L251" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M251" s="33" t="s">
         <v>267</v>
@@ -17006,7 +17006,7 @@
       </c>
       <c r="K252" s="31"/>
       <c r="L252" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M252" s="33" t="s">
         <v>608</v>
@@ -17146,7 +17146,7 @@
       </c>
       <c r="K255" s="31"/>
       <c r="L255" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M255" s="33" t="s">
         <v>611</v>
@@ -17192,7 +17192,7 @@
       </c>
       <c r="K256" s="31"/>
       <c r="L256" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M256" s="33" t="s">
         <v>246</v>
@@ -17286,7 +17286,7 @@
       </c>
       <c r="K258" s="31"/>
       <c r="L258" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M258" s="33" t="s">
         <v>746</v>
@@ -17380,7 +17380,7 @@
       </c>
       <c r="K260" s="31"/>
       <c r="L260" s="31" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="M260" s="33" t="s">
         <v>247</v>
@@ -17428,7 +17428,7 @@
       </c>
       <c r="K261" s="31"/>
       <c r="L261" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M261" s="33" t="s">
         <v>94</v>
@@ -17722,7 +17722,7 @@
       </c>
       <c r="K267" s="31"/>
       <c r="L267" s="31" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="M267" s="33" t="s">
         <v>144</v>
@@ -18080,7 +18080,7 @@
         <v>144</v>
       </c>
       <c r="R274" s="33" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="S274" s="33" t="s">
         <v>643</v>
@@ -18541,7 +18541,7 @@
       <c r="A284" s="34"/>
       <c r="B284" s="34"/>
       <c r="C284" s="34" t="s">
-        <v>753</v>
+        <v>784</v>
       </c>
       <c r="D284" s="31"/>
       <c r="E284" s="31" t="s">
@@ -18603,7 +18603,7 @@
       <c r="A285" s="34"/>
       <c r="B285" s="34"/>
       <c r="C285" s="34" t="s">
-        <v>754</v>
+        <v>785</v>
       </c>
       <c r="D285" s="31"/>
       <c r="E285" s="31" t="s">
@@ -18663,7 +18663,7 @@
       <c r="A286" s="34"/>
       <c r="B286" s="34"/>
       <c r="C286" s="34" t="s">
-        <v>755</v>
+        <v>786</v>
       </c>
       <c r="D286" s="31"/>
       <c r="E286" s="31" t="s">
@@ -18725,15 +18725,15 @@
       <c r="A287" s="34"/>
       <c r="B287" s="34"/>
       <c r="C287" s="34" t="s">
-        <v>758</v>
+        <v>787</v>
       </c>
       <c r="D287" s="31"/>
       <c r="E287" s="31" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="F287" s="31"/>
       <c r="G287" s="31" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="H287" s="31"/>
       <c r="I287" s="33" t="s">
@@ -18823,7 +18823,7 @@
       <c r="A289" s="34"/>
       <c r="B289" s="34"/>
       <c r="C289" s="34" t="s">
-        <v>774</v>
+        <v>788</v>
       </c>
       <c r="D289" s="31"/>
       <c r="E289" s="31" t="s">
@@ -18898,7 +18898,7 @@
       </c>
       <c r="K290" s="31"/>
       <c r="L290" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M290" s="33" t="s">
         <v>102</v>
@@ -18994,7 +18994,7 @@
       </c>
       <c r="K292" s="31"/>
       <c r="L292" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M292" s="33" t="s">
         <v>261</v>
@@ -19036,7 +19036,7 @@
       </c>
       <c r="K293" s="31"/>
       <c r="L293" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M293" s="33" t="s">
         <v>686</v>
@@ -19086,7 +19086,7 @@
       </c>
       <c r="K294" s="31"/>
       <c r="L294" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M294" s="33" t="s">
         <v>261</v>
@@ -19128,7 +19128,7 @@
       </c>
       <c r="K295" s="31"/>
       <c r="L295" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M295" s="33" t="s">
         <v>689</v>
@@ -19178,7 +19178,7 @@
       </c>
       <c r="K296" s="31"/>
       <c r="L296" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M296" s="33" t="s">
         <v>694</v>
@@ -19413,10 +19413,10 @@
       <c r="G301" s="31"/>
       <c r="H301" s="31"/>
       <c r="I301" s="33" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="J301" s="33" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="K301" s="31"/>
       <c r="L301" s="31" t="s">
@@ -19662,7 +19662,7 @@
       </c>
       <c r="K306" s="31"/>
       <c r="L306" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M306" s="33" t="s">
         <v>719</v>
@@ -19946,7 +19946,7 @@
       </c>
       <c r="K312" s="31"/>
       <c r="L312" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M312" s="33" t="s">
         <v>730</v>
@@ -19996,7 +19996,7 @@
       </c>
       <c r="K313" s="31"/>
       <c r="L313" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M313" s="33" t="s">
         <v>731</v>
@@ -20038,7 +20038,7 @@
       </c>
       <c r="K314" s="31"/>
       <c r="L314" s="31" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="M314" s="33" t="s">
         <v>735</v>
@@ -20061,38 +20061,38 @@
     </row>
     <row r="315" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I315" s="37" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="J315" s="37" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="L315" s="37" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="M315" s="37" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
     </row>
     <row r="316" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I316" s="39" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="J316" s="39" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="L316" s="37" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="M316" s="37" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
     </row>
     <row r="317" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I317" s="37" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="J317" s="37" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="L317" s="31" t="s">
         <v>207</v>
@@ -20118,13 +20118,13 @@
     </row>
     <row r="318" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I318" s="37" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="J318" s="37" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="L318" s="37" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="M318" s="37" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
Updating crosswalk to include upcoming newly utilized OITHSPP category in FMWT/STN
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D480E932-2381-4905-BFB6-C496808F6532}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B1328A-8B17-4455-AD0C-3E1DB53A2320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3414" uniqueCount="790">
   <si>
     <t>ACARTELA</t>
   </si>
@@ -3923,9 +3923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
+      <selection pane="bottomLeft" activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5648,9 +5648,13 @@
         <v>70</v>
       </c>
       <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
+      <c r="D28" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
+      <c r="F28" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="G28" s="31"/>
       <c r="H28" s="31" t="s">
         <v>485</v>
@@ -5692,7 +5696,9 @@
         <v>2007</v>
       </c>
       <c r="W28" s="31"/>
-      <c r="X28" s="31"/>
+      <c r="X28" s="31">
+        <v>1980</v>
+      </c>
       <c r="Y28" s="31"/>
       <c r="Z28" s="31">
         <v>1995</v>

</xml_diff>

<commit_message>
Fixed crosswalk to resolve error where the `Zoopsynther` community option was not resolving Acanthocyclops correctly
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24923"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltacouncil.sharepoint.com/sites/Extranet-Science/Shared Documents/NCEAS-DSP working group/Data taskforce/Zooplankton/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="774" documentId="8_{F3296FDE-B87E-414E-85EC-772589208466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E825721-B155-42BB-9EC6-6CBC31CB9BC9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B9F4AC-A813-44D5-9BEC-A5614F7DD47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="911">
   <si>
     <t>Taxname</t>
   </si>
@@ -2863,7 +2863,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3403,7 +3403,7 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" style="12" customWidth="1"/>
     <col min="2" max="2" width="22" style="5" customWidth="1"/>
@@ -3413,7 +3413,7 @@
     <col min="7" max="7" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -3428,7 +3428,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>9</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="28" customFormat="1">
+    <row r="11" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>21</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="28" customFormat="1">
+    <row r="12" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>22</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="28" customFormat="1">
+    <row r="13" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>25</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="28" customFormat="1">
+    <row r="14" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>27</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>28</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>31</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>32</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>33</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>36</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>39</v>
       </c>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1">
+    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>41</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>43</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>45</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>47</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>49</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>51</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>52</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>55</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>58</v>
       </c>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>60</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>63</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>65</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>68</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>71</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>73</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>75</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>78</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16.5" customHeight="1">
+    <row r="38" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>80</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>82</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>85</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>88</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>91</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>94</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>96</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>99</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>100</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>102</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>104</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>107</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>108</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>110</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>113</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>116</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>119</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>121</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>122</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>125</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>128</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>131</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>132</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>135</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>138</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>141</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>143</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
         <v>146</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
         <v>149</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>152</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>154</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>156</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
         <v>157</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>158</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>159</v>
       </c>
@@ -4301,11 +4301,11 @@
   <dimension ref="A1:AD380"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="22" style="37" customWidth="1"/>
     <col min="4" max="7" width="20.28515625" style="37" customWidth="1"/>
@@ -4333,7 +4333,7 @@
     <col min="31" max="16384" width="9.140625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
         <v>160</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15">
+    <row r="2" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -4471,7 +4471,7 @@
       <c r="AC2" s="31"/>
       <c r="AD2" s="31"/>
     </row>
-    <row r="3" spans="1:30" ht="15">
+    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
@@ -4521,7 +4521,7 @@
       <c r="AC3" s="31"/>
       <c r="AD3" s="31"/>
     </row>
-    <row r="4" spans="1:30" ht="15">
+    <row r="4" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -4573,7 +4573,7 @@
       <c r="AC4" s="31"/>
       <c r="AD4" s="31"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -4619,7 +4619,7 @@
       <c r="AC5" s="31"/>
       <c r="AD5" s="31"/>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="31"/>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
@@ -4673,7 +4673,7 @@
       <c r="AC6" s="31"/>
       <c r="AD6" s="31"/>
     </row>
-    <row r="7" spans="1:30" ht="15">
+    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="31"/>
       <c r="C7" s="31"/>
@@ -4719,7 +4719,7 @@
       <c r="AC7" s="31"/>
       <c r="AD7" s="31"/>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="31"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
@@ -4761,7 +4761,7 @@
       <c r="AC8" s="31"/>
       <c r="AD8" s="31"/>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="31"/>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
@@ -4804,7 +4804,7 @@
       </c>
       <c r="AD9" s="31"/>
     </row>
-    <row r="10" spans="1:30" ht="15">
+    <row r="10" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -4848,7 +4848,7 @@
       <c r="AC10" s="31"/>
       <c r="AD10" s="31"/>
     </row>
-    <row r="11" spans="1:30" ht="15">
+    <row r="11" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
@@ -4896,7 +4896,7 @@
       <c r="AC11" s="31"/>
       <c r="AD11" s="31"/>
     </row>
-    <row r="12" spans="1:30" ht="15">
+    <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
@@ -4944,7 +4944,7 @@
       <c r="AC12" s="31"/>
       <c r="AD12" s="31"/>
     </row>
-    <row r="13" spans="1:30" ht="15">
+    <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
       <c r="B13" s="31"/>
       <c r="C13" s="31"/>
@@ -4994,7 +4994,7 @@
       <c r="AC13" s="31"/>
       <c r="AD13" s="31"/>
     </row>
-    <row r="14" spans="1:30" ht="15">
+    <row r="14" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -5044,7 +5044,7 @@
       <c r="AC14" s="31"/>
       <c r="AD14" s="31"/>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
       <c r="B15" s="32" t="s">
         <v>111</v>
@@ -5114,7 +5114,7 @@
       <c r="AC15" s="31"/>
       <c r="AD15" s="31"/>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -5164,7 +5164,7 @@
       <c r="AC16" s="31"/>
       <c r="AD16" s="31"/>
     </row>
-    <row r="17" spans="1:30" ht="15">
+    <row r="17" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -5214,7 +5214,7 @@
       <c r="AC17" s="31"/>
       <c r="AD17" s="31"/>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -5260,7 +5260,7 @@
       <c r="AC18" s="31"/>
       <c r="AD18" s="31"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -5310,7 +5310,7 @@
       <c r="AC19" s="31"/>
       <c r="AD19" s="31"/>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
@@ -5360,7 +5360,7 @@
       <c r="AC20" s="31"/>
       <c r="AD20" s="31"/>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -5410,7 +5410,7 @@
       <c r="AC21" s="31"/>
       <c r="AD21" s="31"/>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -5460,7 +5460,7 @@
       <c r="AC22" s="31"/>
       <c r="AD22" s="31"/>
     </row>
-    <row r="23" spans="1:30" ht="15">
+    <row r="23" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
@@ -5510,7 +5510,7 @@
       <c r="AC23" s="31"/>
       <c r="AD23" s="31"/>
     </row>
-    <row r="24" spans="1:30" ht="15">
+    <row r="24" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
@@ -5560,7 +5560,7 @@
       <c r="AC24" s="31"/>
       <c r="AD24" s="31"/>
     </row>
-    <row r="25" spans="1:30" ht="15">
+    <row r="25" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
@@ -5610,7 +5610,7 @@
       <c r="AC25" s="31"/>
       <c r="AD25" s="31"/>
     </row>
-    <row r="26" spans="1:30" ht="15">
+    <row r="26" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26" s="31"/>
       <c r="C26" s="31"/>
@@ -5660,7 +5660,7 @@
       <c r="AC26" s="31"/>
       <c r="AD26" s="31"/>
     </row>
-    <row r="27" spans="1:30" ht="15">
+    <row r="27" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -5710,7 +5710,7 @@
       <c r="AC27" s="31"/>
       <c r="AD27" s="31"/>
     </row>
-    <row r="28" spans="1:30" ht="15">
+    <row r="28" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -5760,7 +5760,7 @@
       <c r="AC28" s="31"/>
       <c r="AD28" s="31"/>
     </row>
-    <row r="29" spans="1:30" ht="15">
+    <row r="29" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
@@ -5810,7 +5810,7 @@
       <c r="AC29" s="31"/>
       <c r="AD29" s="31"/>
     </row>
-    <row r="30" spans="1:30" ht="15">
+    <row r="30" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -5860,7 +5860,7 @@
       <c r="AC30" s="31"/>
       <c r="AD30" s="31"/>
     </row>
-    <row r="31" spans="1:30" ht="15">
+    <row r="31" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
@@ -5912,7 +5912,7 @@
       <c r="AC31" s="31"/>
       <c r="AD31" s="31"/>
     </row>
-    <row r="32" spans="1:30" ht="15">
+    <row r="32" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="31"/>
       <c r="C32" s="31"/>
@@ -5962,7 +5962,7 @@
       <c r="AC32" s="31"/>
       <c r="AD32" s="31"/>
     </row>
-    <row r="33" spans="1:30" ht="15">
+    <row r="33" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="31"/>
       <c r="C33" s="31"/>
@@ -6012,7 +6012,7 @@
       <c r="AC33" s="31"/>
       <c r="AD33" s="31"/>
     </row>
-    <row r="34" spans="1:30" ht="15">
+    <row r="34" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
@@ -6062,7 +6062,7 @@
       <c r="AC34" s="31"/>
       <c r="AD34" s="31"/>
     </row>
-    <row r="35" spans="1:30" ht="15">
+    <row r="35" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
@@ -6114,7 +6114,7 @@
       <c r="AC35" s="31"/>
       <c r="AD35" s="31"/>
     </row>
-    <row r="36" spans="1:30" ht="15">
+    <row r="36" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
@@ -6164,7 +6164,7 @@
       <c r="AC36" s="31"/>
       <c r="AD36" s="31"/>
     </row>
-    <row r="37" spans="1:30" ht="15">
+    <row r="37" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="31"/>
       <c r="C37" s="31"/>
@@ -6214,7 +6214,7 @@
       <c r="AC37" s="31"/>
       <c r="AD37" s="31"/>
     </row>
-    <row r="38" spans="1:30" ht="15">
+    <row r="38" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="31"/>
       <c r="C38" s="31"/>
@@ -6264,7 +6264,7 @@
       <c r="AC38" s="31"/>
       <c r="AD38" s="31"/>
     </row>
-    <row r="39" spans="1:30" ht="15">
+    <row r="39" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -6314,7 +6314,7 @@
       <c r="AC39" s="31"/>
       <c r="AD39" s="31"/>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="32"/>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
@@ -6370,7 +6370,7 @@
       <c r="AC40" s="31"/>
       <c r="AD40" s="31"/>
     </row>
-    <row r="41" spans="1:30" ht="15">
+    <row r="41" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="B41" s="31"/>
       <c r="C41" s="31"/>
@@ -6419,7 +6419,7 @@
       <c r="AC41" s="31"/>
       <c r="AD41" s="31"/>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="32"/>
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>
@@ -6468,7 +6468,7 @@
       <c r="AC42" s="31"/>
       <c r="AD42" s="31"/>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="32"/>
       <c r="B43" s="32" t="s">
         <v>123</v>
@@ -6530,7 +6530,7 @@
       <c r="AC43" s="31"/>
       <c r="AD43" s="31"/>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="32"/>
       <c r="B44" s="32" t="s">
         <v>114</v>
@@ -6595,7 +6595,7 @@
       <c r="AC44" s="31"/>
       <c r="AD44" s="31"/>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="32"/>
       <c r="B45" s="32" t="s">
         <v>117</v>
@@ -6658,7 +6658,7 @@
       <c r="AC45" s="31"/>
       <c r="AD45" s="31"/>
     </row>
-    <row r="46" spans="1:30" ht="15">
+    <row r="46" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="31"/>
       <c r="B46" s="31"/>
       <c r="C46" s="31"/>
@@ -6710,7 +6710,7 @@
       <c r="AC46" s="31"/>
       <c r="AD46" s="31"/>
     </row>
-    <row r="47" spans="1:30" ht="15">
+    <row r="47" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="31"/>
       <c r="C47" s="31"/>
@@ -6762,7 +6762,7 @@
       <c r="AC47" s="31"/>
       <c r="AD47" s="31"/>
     </row>
-    <row r="48" spans="1:30" ht="15">
+    <row r="48" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
       <c r="C48" s="31"/>
@@ -6814,7 +6814,7 @@
       <c r="AC48" s="31"/>
       <c r="AD48" s="31"/>
     </row>
-    <row r="49" spans="1:30" ht="15">
+    <row r="49" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="31"/>
       <c r="C49" s="31"/>
@@ -6866,7 +6866,7 @@
       <c r="AC49" s="31"/>
       <c r="AD49" s="31"/>
     </row>
-    <row r="50" spans="1:30" ht="15">
+    <row r="50" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="31"/>
       <c r="C50" s="31"/>
@@ -6916,7 +6916,7 @@
       <c r="AC50" s="31"/>
       <c r="AD50" s="31"/>
     </row>
-    <row r="51" spans="1:30" ht="15">
+    <row r="51" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
@@ -6968,7 +6968,7 @@
       <c r="AC51" s="31"/>
       <c r="AD51" s="31"/>
     </row>
-    <row r="52" spans="1:30" ht="15">
+    <row r="52" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
@@ -7017,7 +7017,7 @@
       <c r="AC52" s="31"/>
       <c r="AD52" s="31"/>
     </row>
-    <row r="53" spans="1:30" ht="15">
+    <row r="53" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
@@ -7069,7 +7069,7 @@
       <c r="AC53" s="31"/>
       <c r="AD53" s="31"/>
     </row>
-    <row r="54" spans="1:30" ht="15">
+    <row r="54" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
@@ -7121,7 +7121,7 @@
       <c r="AC54" s="31"/>
       <c r="AD54" s="31"/>
     </row>
-    <row r="55" spans="1:30">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="31"/>
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
@@ -7171,7 +7171,7 @@
       <c r="AC55" s="31"/>
       <c r="AD55" s="31"/>
     </row>
-    <row r="56" spans="1:30">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="31"/>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
@@ -7221,7 +7221,7 @@
       <c r="AC56" s="31"/>
       <c r="AD56" s="31"/>
     </row>
-    <row r="57" spans="1:30" ht="15">
+    <row r="57" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="31"/>
       <c r="B57" s="31"/>
       <c r="C57" s="31"/>
@@ -7267,7 +7267,7 @@
       <c r="AC57" s="31"/>
       <c r="AD57" s="31"/>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="32"/>
       <c r="B58" s="32" t="s">
         <v>8</v>
@@ -7335,7 +7335,7 @@
       <c r="AC58" s="31"/>
       <c r="AD58" s="31"/>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="32"/>
       <c r="B59" s="32"/>
       <c r="C59" s="32"/>
@@ -7385,7 +7385,7 @@
       <c r="AC59" s="31"/>
       <c r="AD59" s="31"/>
     </row>
-    <row r="60" spans="1:30">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="32"/>
       <c r="B60" s="32" t="s">
         <v>5</v>
@@ -7457,7 +7457,7 @@
       <c r="AC60" s="31"/>
       <c r="AD60" s="31"/>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="31"/>
       <c r="B61" s="31"/>
       <c r="C61" s="31"/>
@@ -7509,7 +7509,7 @@
       <c r="AC61" s="31"/>
       <c r="AD61" s="31"/>
     </row>
-    <row r="62" spans="1:30" ht="15">
+    <row r="62" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="31"/>
       <c r="B62" s="31"/>
       <c r="C62" s="31"/>
@@ -7561,7 +7561,7 @@
       <c r="AC62" s="31"/>
       <c r="AD62" s="31"/>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="32"/>
       <c r="B63" s="32"/>
       <c r="C63" s="32"/>
@@ -7611,7 +7611,7 @@
       <c r="AC63" s="31"/>
       <c r="AD63" s="31"/>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
       <c r="B64" s="32"/>
       <c r="C64" s="32"/>
@@ -7663,7 +7663,7 @@
       <c r="AC64" s="31"/>
       <c r="AD64" s="31"/>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" s="32"/>
       <c r="B65" s="32" t="s">
         <v>64</v>
@@ -7719,7 +7719,7 @@
       <c r="AC65" s="31"/>
       <c r="AD65" s="31"/>
     </row>
-    <row r="66" spans="1:30" ht="15">
+    <row r="66" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="31"/>
       <c r="B66" s="31"/>
       <c r="C66" s="31"/>
@@ -7771,7 +7771,7 @@
       <c r="AC66" s="31"/>
       <c r="AD66" s="31"/>
     </row>
-    <row r="67" spans="1:30" ht="15">
+    <row r="67" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="31"/>
       <c r="B67" s="31"/>
       <c r="C67" s="31"/>
@@ -7823,7 +7823,7 @@
       <c r="AC67" s="31"/>
       <c r="AD67" s="31"/>
     </row>
-    <row r="68" spans="1:30">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" s="32"/>
       <c r="B68" s="32"/>
       <c r="C68" s="32"/>
@@ -7877,7 +7877,7 @@
       <c r="AC68" s="31"/>
       <c r="AD68" s="31"/>
     </row>
-    <row r="69" spans="1:30">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" s="31"/>
       <c r="B69" s="31"/>
       <c r="C69" s="31"/>
@@ -7931,7 +7931,7 @@
       <c r="AC69" s="31"/>
       <c r="AD69" s="31"/>
     </row>
-    <row r="70" spans="1:30">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" s="32"/>
       <c r="B70" s="32" t="s">
         <v>14</v>
@@ -8001,7 +8001,7 @@
       <c r="AC70" s="31"/>
       <c r="AD70" s="31"/>
     </row>
-    <row r="71" spans="1:30">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" s="32"/>
       <c r="B71" s="32" t="s">
         <v>61</v>
@@ -8071,7 +8071,7 @@
       <c r="AC71" s="31"/>
       <c r="AD71" s="31"/>
     </row>
-    <row r="72" spans="1:30">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" s="32"/>
       <c r="B72" s="32"/>
       <c r="C72" s="32"/>
@@ -8121,7 +8121,7 @@
       <c r="AC72" s="31"/>
       <c r="AD72" s="31"/>
     </row>
-    <row r="73" spans="1:30" ht="15">
+    <row r="73" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="31"/>
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
@@ -8173,7 +8173,7 @@
       <c r="AC73" s="31"/>
       <c r="AD73" s="31"/>
     </row>
-    <row r="74" spans="1:30" ht="15">
+    <row r="74" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="31"/>
       <c r="B74" s="31"/>
       <c r="C74" s="31"/>
@@ -8225,7 +8225,7 @@
       <c r="AC74" s="31"/>
       <c r="AD74" s="31"/>
     </row>
-    <row r="75" spans="1:30" ht="15">
+    <row r="75" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="31"/>
       <c r="B75" s="31"/>
       <c r="C75" s="31"/>
@@ -8275,7 +8275,7 @@
       <c r="AC75" s="31"/>
       <c r="AD75" s="31"/>
     </row>
-    <row r="76" spans="1:30" ht="15">
+    <row r="76" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="31"/>
       <c r="B76" s="31"/>
       <c r="C76" s="31"/>
@@ -8327,7 +8327,7 @@
       <c r="AC76" s="31"/>
       <c r="AD76" s="31"/>
     </row>
-    <row r="77" spans="1:30">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" s="32"/>
       <c r="B77" s="32"/>
       <c r="C77" s="32"/>
@@ -8387,7 +8387,7 @@
       <c r="AC77" s="31"/>
       <c r="AD77" s="31"/>
     </row>
-    <row r="78" spans="1:30">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" s="32"/>
       <c r="B78" s="32"/>
       <c r="C78" s="32"/>
@@ -8437,7 +8437,7 @@
       <c r="AC78" s="31"/>
       <c r="AD78" s="31"/>
     </row>
-    <row r="79" spans="1:30">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" s="32"/>
       <c r="B79" s="32"/>
       <c r="C79" s="32"/>
@@ -8497,7 +8497,7 @@
       <c r="AC79" s="31"/>
       <c r="AD79" s="31"/>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" s="32"/>
       <c r="B80" s="32" t="s">
         <v>23</v>
@@ -8569,7 +8569,7 @@
       <c r="AC80" s="31"/>
       <c r="AD80" s="31"/>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" s="32"/>
       <c r="B81" s="32"/>
       <c r="C81" s="32"/>
@@ -8621,7 +8621,7 @@
       <c r="AC81" s="31"/>
       <c r="AD81" s="31"/>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" s="32"/>
       <c r="B82" s="32" t="s">
         <v>29</v>
@@ -8693,7 +8693,7 @@
       <c r="AC82" s="31"/>
       <c r="AD82" s="31"/>
     </row>
-    <row r="83" spans="1:30">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" s="32"/>
       <c r="B83" s="32"/>
       <c r="C83" s="32"/>
@@ -8745,7 +8745,7 @@
       <c r="AC83" s="31"/>
       <c r="AD83" s="31"/>
     </row>
-    <row r="84" spans="1:30">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" s="32"/>
       <c r="B84" s="32"/>
       <c r="C84" s="32"/>
@@ -8797,7 +8797,7 @@
       <c r="AC84" s="31"/>
       <c r="AD84" s="31"/>
     </row>
-    <row r="85" spans="1:30" ht="15">
+    <row r="85" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="31"/>
       <c r="B85" s="31"/>
       <c r="C85" s="31"/>
@@ -8849,7 +8849,7 @@
       <c r="AC85" s="31"/>
       <c r="AD85" s="31"/>
     </row>
-    <row r="86" spans="1:30" ht="15">
+    <row r="86" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="31"/>
       <c r="B86" s="31"/>
       <c r="C86" s="31"/>
@@ -8899,7 +8899,7 @@
       <c r="AC86" s="31"/>
       <c r="AD86" s="31"/>
     </row>
-    <row r="87" spans="1:30">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" s="32"/>
       <c r="B87" s="32" t="s">
         <v>34</v>
@@ -8969,7 +8969,7 @@
       <c r="AC87" s="31"/>
       <c r="AD87" s="31"/>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" s="32"/>
       <c r="B88" s="32"/>
       <c r="C88" s="32"/>
@@ -9019,7 +9019,7 @@
       <c r="AC88" s="31"/>
       <c r="AD88" s="31"/>
     </row>
-    <row r="89" spans="1:30">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" s="32"/>
       <c r="B89" s="32" t="s">
         <v>19</v>
@@ -9081,7 +9081,7 @@
       <c r="AC89" s="31"/>
       <c r="AD89" s="31"/>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" s="31"/>
       <c r="B90" s="31" t="s">
         <v>76</v>
@@ -9147,7 +9147,7 @@
       <c r="AC90" s="31"/>
       <c r="AD90" s="31"/>
     </row>
-    <row r="91" spans="1:30">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" s="32"/>
       <c r="B91" s="32"/>
       <c r="C91" s="32"/>
@@ -9201,7 +9201,7 @@
       <c r="AC91" s="31"/>
       <c r="AD91" s="31"/>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="31"/>
       <c r="B92" s="31" t="s">
         <v>74</v>
@@ -9267,7 +9267,7 @@
       <c r="AC92" s="31"/>
       <c r="AD92" s="31"/>
     </row>
-    <row r="93" spans="1:30">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" s="31"/>
       <c r="B93" s="31" t="s">
         <v>59</v>
@@ -9325,7 +9325,7 @@
       <c r="AC93" s="31"/>
       <c r="AD93" s="31"/>
     </row>
-    <row r="94" spans="1:30">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" s="32"/>
       <c r="B94" s="32" t="s">
         <v>11</v>
@@ -9385,7 +9385,7 @@
       <c r="AC94" s="31"/>
       <c r="AD94" s="31"/>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" s="31"/>
       <c r="B95" s="31" t="s">
         <v>81</v>
@@ -9445,7 +9445,7 @@
       <c r="AC95" s="31"/>
       <c r="AD95" s="31"/>
     </row>
-    <row r="96" spans="1:30">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" s="31"/>
       <c r="B96" s="31"/>
       <c r="C96" s="31"/>
@@ -9501,7 +9501,7 @@
       <c r="AC96" s="31"/>
       <c r="AD96" s="31"/>
     </row>
-    <row r="97" spans="1:30">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" s="32" t="s">
         <v>101</v>
       </c>
@@ -9563,7 +9563,7 @@
       <c r="AC97" s="31"/>
       <c r="AD97" s="31"/>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" s="32"/>
       <c r="B98" s="32" t="s">
         <v>66</v>
@@ -9631,7 +9631,7 @@
       <c r="AC98" s="31"/>
       <c r="AD98" s="31"/>
     </row>
-    <row r="99" spans="1:30">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99" s="32" t="s">
         <v>105</v>
       </c>
@@ -9701,7 +9701,7 @@
       <c r="AC99" s="31"/>
       <c r="AD99" s="31"/>
     </row>
-    <row r="100" spans="1:30">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100" s="32"/>
       <c r="B100" s="32"/>
       <c r="C100" s="32"/>
@@ -9757,7 +9757,7 @@
       <c r="AC100" s="31"/>
       <c r="AD100" s="31"/>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" s="32"/>
       <c r="B101" s="32" t="s">
         <v>26</v>
@@ -9827,7 +9827,7 @@
       <c r="AC101" s="31"/>
       <c r="AD101" s="31"/>
     </row>
-    <row r="102" spans="1:30">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102" s="32"/>
       <c r="B102" s="32" t="s">
         <v>69</v>
@@ -9895,7 +9895,7 @@
       <c r="AC102" s="31"/>
       <c r="AD102" s="31"/>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A103" s="32"/>
       <c r="B103" s="32"/>
       <c r="C103" s="32"/>
@@ -9949,7 +9949,7 @@
       <c r="AC103" s="31"/>
       <c r="AD103" s="31"/>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104" s="32" t="s">
         <v>109</v>
       </c>
@@ -10017,7 +10017,7 @@
       <c r="AC104" s="31"/>
       <c r="AD104" s="31"/>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A105" s="31"/>
       <c r="B105" s="31" t="s">
         <v>83</v>
@@ -10085,7 +10085,7 @@
       <c r="AC105" s="31"/>
       <c r="AD105" s="31"/>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" s="32"/>
       <c r="B106" s="32"/>
       <c r="C106" s="32"/>
@@ -10147,7 +10147,7 @@
       </c>
       <c r="AD106" s="31"/>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107" s="32"/>
       <c r="B107" s="32"/>
       <c r="C107" s="32"/>
@@ -10203,7 +10203,7 @@
       <c r="AC107" s="31"/>
       <c r="AD107" s="31"/>
     </row>
-    <row r="108" spans="1:30">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L108" s="31" t="s">
         <v>13</v>
       </c>
@@ -10238,7 +10238,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:30">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L109" s="41" t="s">
         <v>28</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="110" spans="1:30">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L110" s="41" t="s">
         <v>22</v>
       </c>
@@ -10314,7 +10314,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="111" spans="1:30">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A111" s="32"/>
       <c r="B111" s="32" t="s">
         <v>357</v>
@@ -10374,7 +10374,7 @@
       <c r="AC111" s="31"/>
       <c r="AD111" s="31"/>
     </row>
-    <row r="112" spans="1:30">
+    <row r="112" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A112" s="32"/>
       <c r="B112" s="32"/>
       <c r="C112" s="32"/>
@@ -10426,19 +10426,13 @@
       <c r="AC112" s="31"/>
       <c r="AD112" s="31"/>
     </row>
-    <row r="113" spans="1:30">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A113" s="32"/>
-      <c r="B113" s="32" t="s">
-        <v>37</v>
-      </c>
+      <c r="B113" s="32"/>
       <c r="C113" s="32"/>
-      <c r="D113" s="32" t="s">
-        <v>37</v>
-      </c>
+      <c r="D113" s="32"/>
       <c r="E113" s="32"/>
-      <c r="F113" s="32" t="s">
-        <v>37</v>
-      </c>
+      <c r="F113" s="32"/>
       <c r="G113" s="32"/>
       <c r="H113" s="31" t="s">
         <v>38</v>
@@ -10500,7 +10494,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="114" spans="1:30">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A114" s="32"/>
       <c r="B114" s="32" t="s">
         <v>53</v>
@@ -10564,7 +10558,7 @@
       <c r="AC114" s="31"/>
       <c r="AD114" s="31"/>
     </row>
-    <row r="115" spans="1:30">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A115" s="31"/>
       <c r="B115" s="31"/>
       <c r="C115" s="31"/>
@@ -10614,7 +10608,7 @@
       <c r="AC115" s="31"/>
       <c r="AD115" s="31"/>
     </row>
-    <row r="116" spans="1:30">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A116" s="32" t="s">
         <v>86</v>
       </c>
@@ -10676,7 +10670,7 @@
       <c r="AC116" s="31"/>
       <c r="AD116" s="31"/>
     </row>
-    <row r="117" spans="1:30" ht="15">
+    <row r="117" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="31"/>
       <c r="B117" s="31"/>
       <c r="C117" s="31"/>
@@ -10726,7 +10720,7 @@
       <c r="AC117" s="31"/>
       <c r="AD117" s="31"/>
     </row>
-    <row r="118" spans="1:30" ht="15">
+    <row r="118" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="31"/>
       <c r="B118" s="31"/>
       <c r="C118" s="31"/>
@@ -10782,7 +10776,7 @@
       <c r="AC118" s="31"/>
       <c r="AD118" s="31"/>
     </row>
-    <row r="119" spans="1:30" ht="15">
+    <row r="119" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="31"/>
       <c r="B119" s="31"/>
       <c r="C119" s="31"/>
@@ -10834,7 +10828,7 @@
       <c r="AC119" s="31"/>
       <c r="AD119" s="31"/>
     </row>
-    <row r="120" spans="1:30" ht="15">
+    <row r="120" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="31"/>
       <c r="B120" s="31"/>
       <c r="C120" s="31"/>
@@ -10886,7 +10880,7 @@
       <c r="AC120" s="31"/>
       <c r="AD120" s="31"/>
     </row>
-    <row r="121" spans="1:30" ht="15">
+    <row r="121" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="31"/>
       <c r="B121" s="31"/>
       <c r="C121" s="31"/>
@@ -10936,7 +10930,7 @@
       <c r="AC121" s="31"/>
       <c r="AD121" s="31"/>
     </row>
-    <row r="122" spans="1:30" ht="15">
+    <row r="122" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="31"/>
       <c r="B122" s="31"/>
       <c r="C122" s="31"/>
@@ -10986,7 +10980,7 @@
       <c r="AC122" s="31"/>
       <c r="AD122" s="31"/>
     </row>
-    <row r="123" spans="1:30" ht="15">
+    <row r="123" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="31"/>
       <c r="B123" s="31"/>
       <c r="C123" s="31"/>
@@ -11038,7 +11032,7 @@
       <c r="AC123" s="31"/>
       <c r="AD123" s="31"/>
     </row>
-    <row r="124" spans="1:30" ht="15">
+    <row r="124" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="31"/>
       <c r="B124" s="31"/>
       <c r="C124" s="31"/>
@@ -11090,7 +11084,7 @@
       <c r="AC124" s="31"/>
       <c r="AD124" s="31"/>
     </row>
-    <row r="125" spans="1:30" ht="15">
+    <row r="125" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="31"/>
       <c r="B125" s="31"/>
       <c r="C125" s="31"/>
@@ -11142,7 +11136,7 @@
       <c r="AC125" s="31"/>
       <c r="AD125" s="31"/>
     </row>
-    <row r="126" spans="1:30" ht="15">
+    <row r="126" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="31"/>
       <c r="B126" s="31"/>
       <c r="C126" s="31"/>
@@ -11194,7 +11188,7 @@
       <c r="AC126" s="31"/>
       <c r="AD126" s="31"/>
     </row>
-    <row r="127" spans="1:30" ht="15">
+    <row r="127" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="31"/>
       <c r="B127" s="31"/>
       <c r="C127" s="31"/>
@@ -11246,7 +11240,7 @@
       <c r="AC127" s="31"/>
       <c r="AD127" s="31"/>
     </row>
-    <row r="128" spans="1:30" ht="15">
+    <row r="128" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="31"/>
       <c r="B128" s="31"/>
       <c r="C128" s="31"/>
@@ -11300,7 +11294,7 @@
       <c r="AC128" s="31"/>
       <c r="AD128" s="31"/>
     </row>
-    <row r="129" spans="1:30">
+    <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129" s="31"/>
       <c r="B129" s="31"/>
       <c r="C129" s="31"/>
@@ -11350,7 +11344,7 @@
       <c r="AC129" s="31"/>
       <c r="AD129" s="31"/>
     </row>
-    <row r="130" spans="1:30">
+    <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130" s="31" t="s">
         <v>42</v>
       </c>
@@ -11424,7 +11418,7 @@
       <c r="AC130" s="31"/>
       <c r="AD130" s="31"/>
     </row>
-    <row r="131" spans="1:30">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131" s="32" t="s">
         <v>40</v>
       </c>
@@ -11494,7 +11488,7 @@
       <c r="AC131" s="31"/>
       <c r="AD131" s="31"/>
     </row>
-    <row r="132" spans="1:30">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132" s="32" t="s">
         <v>89</v>
       </c>
@@ -11562,7 +11556,7 @@
       <c r="AC132" s="31"/>
       <c r="AD132" s="31"/>
     </row>
-    <row r="133" spans="1:30">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133" s="31" t="s">
         <v>44</v>
       </c>
@@ -11636,7 +11630,7 @@
       <c r="AC133" s="31"/>
       <c r="AD133" s="31"/>
     </row>
-    <row r="134" spans="1:30" ht="15">
+    <row r="134" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="31"/>
       <c r="B134" s="31"/>
       <c r="C134" s="31"/>
@@ -11688,7 +11682,7 @@
       <c r="AC134" s="31"/>
       <c r="AD134" s="31"/>
     </row>
-    <row r="135" spans="1:30">
+    <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135" s="31"/>
       <c r="B135" s="31"/>
       <c r="C135" s="31"/>
@@ -11742,7 +11736,7 @@
       <c r="AC135" s="31"/>
       <c r="AD135" s="31"/>
     </row>
-    <row r="136" spans="1:30" ht="15">
+    <row r="136" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="31"/>
       <c r="B136" s="31"/>
       <c r="C136" s="31"/>
@@ -11794,7 +11788,7 @@
       <c r="AC136" s="31"/>
       <c r="AD136" s="31"/>
     </row>
-    <row r="137" spans="1:30" ht="15">
+    <row r="137" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="31"/>
       <c r="B137" s="31"/>
       <c r="C137" s="31"/>
@@ -11846,7 +11840,7 @@
       <c r="AC137" s="31"/>
       <c r="AD137" s="31"/>
     </row>
-    <row r="138" spans="1:30" ht="15">
+    <row r="138" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="31"/>
       <c r="B138" s="31"/>
       <c r="C138" s="31"/>
@@ -11896,7 +11890,7 @@
       <c r="AC138" s="31"/>
       <c r="AD138" s="31"/>
     </row>
-    <row r="139" spans="1:30">
+    <row r="139" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A139" s="32" t="s">
         <v>46</v>
       </c>
@@ -11970,7 +11964,7 @@
       <c r="AC139" s="31"/>
       <c r="AD139" s="31"/>
     </row>
-    <row r="140" spans="1:30">
+    <row r="140" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A140" s="32" t="s">
         <v>48</v>
       </c>
@@ -12042,7 +12036,7 @@
       <c r="AC140" s="31"/>
       <c r="AD140" s="31"/>
     </row>
-    <row r="141" spans="1:30">
+    <row r="141" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A141" s="31" t="s">
         <v>50</v>
       </c>
@@ -12112,7 +12106,7 @@
       <c r="AC141" s="31"/>
       <c r="AD141" s="31"/>
     </row>
-    <row r="142" spans="1:30">
+    <row r="142" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A142" s="32" t="s">
         <v>92</v>
       </c>
@@ -12178,7 +12172,7 @@
       <c r="AC142" s="31"/>
       <c r="AD142" s="31"/>
     </row>
-    <row r="143" spans="1:30" ht="15">
+    <row r="143" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="31"/>
       <c r="B143" s="31"/>
       <c r="C143" s="31"/>
@@ -12230,7 +12224,7 @@
       <c r="AC143" s="31"/>
       <c r="AD143" s="31"/>
     </row>
-    <row r="144" spans="1:30" ht="15">
+    <row r="144" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="31"/>
       <c r="B144" s="31"/>
       <c r="C144" s="31"/>
@@ -12282,7 +12276,7 @@
       <c r="AC144" s="31"/>
       <c r="AD144" s="31"/>
     </row>
-    <row r="145" spans="1:30" ht="15">
+    <row r="145" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="31"/>
       <c r="B145" s="31"/>
       <c r="C145" s="31"/>
@@ -12334,7 +12328,7 @@
       <c r="AC145" s="31"/>
       <c r="AD145" s="31"/>
     </row>
-    <row r="146" spans="1:30" ht="15">
+    <row r="146" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="31"/>
       <c r="B146" s="31"/>
       <c r="C146" s="31"/>
@@ -12388,7 +12382,7 @@
       <c r="AC146" s="31"/>
       <c r="AD146" s="31"/>
     </row>
-    <row r="147" spans="1:30" ht="15">
+    <row r="147" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="31"/>
       <c r="B147" s="31"/>
       <c r="C147" s="31"/>
@@ -12440,7 +12434,7 @@
       <c r="AC147" s="31"/>
       <c r="AD147" s="31"/>
     </row>
-    <row r="148" spans="1:30" ht="15">
+    <row r="148" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="31"/>
       <c r="B148" s="31"/>
       <c r="C148" s="31"/>
@@ -12490,7 +12484,7 @@
       <c r="AC148" s="31"/>
       <c r="AD148" s="31"/>
     </row>
-    <row r="149" spans="1:30">
+    <row r="149" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A149" s="32" t="s">
         <v>444</v>
       </c>
@@ -12542,7 +12536,7 @@
       <c r="AC149" s="31"/>
       <c r="AD149" s="31"/>
     </row>
-    <row r="150" spans="1:30">
+    <row r="150" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A150" s="32" t="s">
         <v>95</v>
       </c>
@@ -12598,7 +12592,7 @@
       <c r="AC150" s="31"/>
       <c r="AD150" s="31"/>
     </row>
-    <row r="151" spans="1:30" ht="15">
+    <row r="151" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="31"/>
       <c r="B151" s="31"/>
       <c r="C151" s="31"/>
@@ -12650,7 +12644,7 @@
       <c r="AC151" s="31"/>
       <c r="AD151" s="31"/>
     </row>
-    <row r="152" spans="1:30">
+    <row r="152" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A152" s="31"/>
       <c r="B152" s="31"/>
       <c r="C152" s="31"/>
@@ -12702,7 +12696,7 @@
       <c r="AC152" s="31"/>
       <c r="AD152" s="31"/>
     </row>
-    <row r="153" spans="1:30">
+    <row r="153" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A153" s="31"/>
       <c r="B153" s="31"/>
       <c r="C153" s="31"/>
@@ -12754,7 +12748,7 @@
       <c r="AC153" s="31"/>
       <c r="AD153" s="31"/>
     </row>
-    <row r="154" spans="1:30">
+    <row r="154" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L154" s="41" t="s">
         <v>448</v>
       </c>
@@ -12780,7 +12774,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="155" spans="1:30">
+    <row r="155" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L155" s="41" t="s">
         <v>41</v>
       </c>
@@ -12818,7 +12812,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="156" spans="1:30">
+    <row r="156" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A156" s="31" t="s">
         <v>56</v>
       </c>
@@ -12884,7 +12878,7 @@
       <c r="AC156" s="31"/>
       <c r="AD156" s="31"/>
     </row>
-    <row r="157" spans="1:30">
+    <row r="157" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A157" s="31" t="s">
         <v>97</v>
       </c>
@@ -12940,7 +12934,7 @@
       <c r="AC157" s="31"/>
       <c r="AD157" s="31"/>
     </row>
-    <row r="158" spans="1:30">
+    <row r="158" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A158" s="32" t="s">
         <v>103</v>
       </c>
@@ -12998,7 +12992,7 @@
       <c r="AC158" s="31"/>
       <c r="AD158" s="31"/>
     </row>
-    <row r="159" spans="1:30">
+    <row r="159" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A159" s="31"/>
       <c r="B159" s="31"/>
       <c r="C159" s="31"/>
@@ -13044,7 +13038,7 @@
       <c r="AC159" s="31"/>
       <c r="AD159" s="31"/>
     </row>
-    <row r="160" spans="1:30">
+    <row r="160" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A160" s="31"/>
       <c r="B160" s="31"/>
       <c r="C160" s="31"/>
@@ -13090,7 +13084,7 @@
       <c r="AC160" s="31"/>
       <c r="AD160" s="31"/>
     </row>
-    <row r="161" spans="1:30">
+    <row r="161" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L161" s="41" t="s">
         <v>293</v>
       </c>
@@ -13113,7 +13107,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="162" spans="1:30">
+    <row r="162" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A162" s="31"/>
       <c r="B162" s="31"/>
       <c r="C162" s="31"/>
@@ -13163,7 +13157,7 @@
       <c r="AC162" s="31"/>
       <c r="AD162" s="31"/>
     </row>
-    <row r="163" spans="1:30">
+    <row r="163" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A163" s="31"/>
       <c r="B163" s="31"/>
       <c r="C163" s="31"/>
@@ -13213,7 +13207,7 @@
       <c r="AC163" s="31"/>
       <c r="AD163" s="31"/>
     </row>
-    <row r="164" spans="1:30">
+    <row r="164" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A164" s="31"/>
       <c r="B164" s="31"/>
       <c r="C164" s="31"/>
@@ -13263,7 +13257,7 @@
       <c r="AC164" s="31"/>
       <c r="AD164" s="31"/>
     </row>
-    <row r="165" spans="1:30">
+    <row r="165" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A165" s="31"/>
       <c r="B165" s="31"/>
       <c r="C165" s="31"/>
@@ -13313,7 +13307,7 @@
       <c r="AC165" s="31"/>
       <c r="AD165" s="31"/>
     </row>
-    <row r="166" spans="1:30" ht="15">
+    <row r="166" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="31"/>
       <c r="B166" s="31"/>
       <c r="C166" s="31"/>
@@ -13361,7 +13355,7 @@
       <c r="AC166" s="31"/>
       <c r="AD166" s="31"/>
     </row>
-    <row r="167" spans="1:30">
+    <row r="167" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A167" s="31"/>
       <c r="B167" s="31"/>
       <c r="C167" s="31"/>
@@ -13409,7 +13403,7 @@
       <c r="AC167" s="31"/>
       <c r="AD167" s="31"/>
     </row>
-    <row r="168" spans="1:30">
+    <row r="168" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A168" s="31"/>
       <c r="B168" s="31"/>
       <c r="C168" s="31"/>
@@ -13459,7 +13453,7 @@
       <c r="AC168" s="31"/>
       <c r="AD168" s="31"/>
     </row>
-    <row r="169" spans="1:30">
+    <row r="169" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A169" s="31"/>
       <c r="B169" s="31"/>
       <c r="C169" s="31"/>
@@ -13509,7 +13503,7 @@
       <c r="AC169" s="31"/>
       <c r="AD169" s="31"/>
     </row>
-    <row r="170" spans="1:30">
+    <row r="170" spans="1:30" x14ac:dyDescent="0.2">
       <c r="I170" s="37" t="s">
         <v>469</v>
       </c>
@@ -13538,7 +13532,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="171" spans="1:30">
+    <row r="171" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A171" s="31"/>
       <c r="B171" s="31"/>
       <c r="C171" s="31"/>
@@ -13588,7 +13582,7 @@
       <c r="AC171" s="31"/>
       <c r="AD171" s="31"/>
     </row>
-    <row r="172" spans="1:30">
+    <row r="172" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A172" s="31"/>
       <c r="B172" s="31"/>
       <c r="C172" s="31"/>
@@ -13638,7 +13632,7 @@
       <c r="AC172" s="31"/>
       <c r="AD172" s="31"/>
     </row>
-    <row r="173" spans="1:30">
+    <row r="173" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A173" s="31"/>
       <c r="B173" s="31"/>
       <c r="C173" s="31"/>
@@ -13688,7 +13682,7 @@
       <c r="AC173" s="31"/>
       <c r="AD173" s="31"/>
     </row>
-    <row r="174" spans="1:30">
+    <row r="174" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A174" s="31"/>
       <c r="B174" s="31"/>
       <c r="C174" s="31"/>
@@ -13738,7 +13732,7 @@
       <c r="AC174" s="31"/>
       <c r="AD174" s="31"/>
     </row>
-    <row r="175" spans="1:30">
+    <row r="175" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A175" s="31"/>
       <c r="B175" s="31"/>
       <c r="C175" s="31"/>
@@ -13788,7 +13782,7 @@
       <c r="AC175" s="31"/>
       <c r="AD175" s="31"/>
     </row>
-    <row r="176" spans="1:30">
+    <row r="176" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A176" s="31"/>
       <c r="B176" s="31"/>
       <c r="C176" s="31"/>
@@ -13838,7 +13832,7 @@
       <c r="AC176" s="31"/>
       <c r="AD176" s="31"/>
     </row>
-    <row r="177" spans="1:30">
+    <row r="177" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A177" s="31"/>
       <c r="B177" s="31"/>
       <c r="C177" s="31"/>
@@ -13888,7 +13882,7 @@
       <c r="AC177" s="31"/>
       <c r="AD177" s="31"/>
     </row>
-    <row r="178" spans="1:30">
+    <row r="178" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A178" s="31"/>
       <c r="B178" s="31"/>
       <c r="C178" s="31"/>
@@ -13938,7 +13932,7 @@
       <c r="AC178" s="31"/>
       <c r="AD178" s="31"/>
     </row>
-    <row r="179" spans="1:30">
+    <row r="179" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A179" s="31"/>
       <c r="B179" s="31"/>
       <c r="C179" s="31"/>
@@ -13988,7 +13982,7 @@
       <c r="AC179" s="31"/>
       <c r="AD179" s="31"/>
     </row>
-    <row r="180" spans="1:30">
+    <row r="180" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A180" s="31"/>
       <c r="B180" s="31"/>
       <c r="C180" s="31"/>
@@ -14038,7 +14032,7 @@
       <c r="AC180" s="31"/>
       <c r="AD180" s="31"/>
     </row>
-    <row r="181" spans="1:30">
+    <row r="181" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A181" s="31"/>
       <c r="B181" s="31"/>
       <c r="C181" s="31"/>
@@ -14088,7 +14082,7 @@
       <c r="AC181" s="31"/>
       <c r="AD181" s="31"/>
     </row>
-    <row r="182" spans="1:30">
+    <row r="182" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A182" s="31"/>
       <c r="B182" s="31"/>
       <c r="C182" s="31"/>
@@ -14138,7 +14132,7 @@
       <c r="AC182" s="31"/>
       <c r="AD182" s="31"/>
     </row>
-    <row r="183" spans="1:30">
+    <row r="183" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A183" s="31"/>
       <c r="B183" s="31"/>
       <c r="C183" s="31"/>
@@ -14188,7 +14182,7 @@
       <c r="AC183" s="31"/>
       <c r="AD183" s="31"/>
     </row>
-    <row r="184" spans="1:30">
+    <row r="184" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A184" s="31"/>
       <c r="B184" s="31"/>
       <c r="C184" s="31"/>
@@ -14240,7 +14234,7 @@
       <c r="AC184" s="31"/>
       <c r="AD184" s="31"/>
     </row>
-    <row r="185" spans="1:30">
+    <row r="185" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A185" s="31"/>
       <c r="B185" s="31"/>
       <c r="C185" s="31"/>
@@ -14290,7 +14284,7 @@
       <c r="AC185" s="31"/>
       <c r="AD185" s="31"/>
     </row>
-    <row r="186" spans="1:30">
+    <row r="186" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A186" s="31"/>
       <c r="B186" s="31"/>
       <c r="C186" s="31"/>
@@ -14340,7 +14334,7 @@
       <c r="AC186" s="31"/>
       <c r="AD186" s="31"/>
     </row>
-    <row r="187" spans="1:30">
+    <row r="187" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A187" s="31"/>
       <c r="B187" s="31"/>
       <c r="C187" s="31"/>
@@ -14388,7 +14382,7 @@
       <c r="AC187" s="31"/>
       <c r="AD187" s="31"/>
     </row>
-    <row r="188" spans="1:30">
+    <row r="188" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A188" s="31"/>
       <c r="B188" s="31"/>
       <c r="C188" s="31"/>
@@ -14446,7 +14440,7 @@
       </c>
       <c r="AD188" s="31"/>
     </row>
-    <row r="189" spans="1:30" ht="15">
+    <row r="189" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="31"/>
       <c r="B189" s="31"/>
       <c r="C189" s="31"/>
@@ -14496,7 +14490,7 @@
       <c r="AC189" s="31"/>
       <c r="AD189" s="31"/>
     </row>
-    <row r="190" spans="1:30">
+    <row r="190" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A190" s="31"/>
       <c r="B190" s="31"/>
       <c r="C190" s="31"/>
@@ -14546,7 +14540,7 @@
       <c r="AC190" s="31"/>
       <c r="AD190" s="31"/>
     </row>
-    <row r="191" spans="1:30" ht="15">
+    <row r="191" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="31"/>
       <c r="B191" s="31"/>
       <c r="C191" s="31"/>
@@ -14594,7 +14588,7 @@
       <c r="AC191" s="31"/>
       <c r="AD191" s="31"/>
     </row>
-    <row r="192" spans="1:30" ht="15">
+    <row r="192" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="31"/>
       <c r="B192" s="31"/>
       <c r="C192" s="31"/>
@@ -14642,7 +14636,7 @@
       <c r="AC192" s="31"/>
       <c r="AD192" s="31"/>
     </row>
-    <row r="193" spans="1:30" ht="15">
+    <row r="193" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="31"/>
       <c r="B193" s="31"/>
       <c r="C193" s="31"/>
@@ -14690,7 +14684,7 @@
       <c r="AC193" s="31"/>
       <c r="AD193" s="31"/>
     </row>
-    <row r="194" spans="1:30" ht="15">
+    <row r="194" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="31"/>
       <c r="B194" s="31"/>
       <c r="C194" s="31"/>
@@ -14738,7 +14732,7 @@
       <c r="AC194" s="31"/>
       <c r="AD194" s="31"/>
     </row>
-    <row r="195" spans="1:30">
+    <row r="195" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A195" s="31"/>
       <c r="B195" s="31"/>
       <c r="C195" s="31"/>
@@ -14786,7 +14780,7 @@
       <c r="AC195" s="31"/>
       <c r="AD195" s="31"/>
     </row>
-    <row r="196" spans="1:30">
+    <row r="196" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A196" s="31"/>
       <c r="B196" s="31"/>
       <c r="C196" s="31"/>
@@ -14834,7 +14828,7 @@
       <c r="AC196" s="31"/>
       <c r="AD196" s="31"/>
     </row>
-    <row r="197" spans="1:30">
+    <row r="197" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A197" s="31"/>
       <c r="B197" s="31"/>
       <c r="C197" s="31"/>
@@ -14882,7 +14876,7 @@
       <c r="AC197" s="31"/>
       <c r="AD197" s="31"/>
     </row>
-    <row r="198" spans="1:30">
+    <row r="198" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A198" s="31"/>
       <c r="B198" s="31"/>
       <c r="C198" s="31"/>
@@ -14930,7 +14924,7 @@
       <c r="AC198" s="31"/>
       <c r="AD198" s="31"/>
     </row>
-    <row r="199" spans="1:30">
+    <row r="199" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A199" s="31"/>
       <c r="B199" s="31"/>
       <c r="C199" s="31"/>
@@ -14980,7 +14974,7 @@
       <c r="AC199" s="31"/>
       <c r="AD199" s="31"/>
     </row>
-    <row r="200" spans="1:30">
+    <row r="200" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A200" s="31"/>
       <c r="B200" s="31"/>
       <c r="C200" s="31"/>
@@ -15030,7 +15024,7 @@
       <c r="AC200" s="31"/>
       <c r="AD200" s="31"/>
     </row>
-    <row r="201" spans="1:30">
+    <row r="201" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A201" s="31"/>
       <c r="B201" s="31"/>
       <c r="C201" s="31"/>
@@ -15080,7 +15074,7 @@
       <c r="AC201" s="31"/>
       <c r="AD201" s="31"/>
     </row>
-    <row r="202" spans="1:30">
+    <row r="202" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A202" s="31"/>
       <c r="B202" s="31"/>
       <c r="C202" s="31"/>
@@ -15130,7 +15124,7 @@
       <c r="AC202" s="31"/>
       <c r="AD202" s="31"/>
     </row>
-    <row r="203" spans="1:30">
+    <row r="203" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A203" s="31"/>
       <c r="B203" s="31"/>
       <c r="C203" s="31"/>
@@ -15180,7 +15174,7 @@
       <c r="AC203" s="31"/>
       <c r="AD203" s="31"/>
     </row>
-    <row r="204" spans="1:30">
+    <row r="204" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A204" s="31"/>
       <c r="B204" s="31"/>
       <c r="C204" s="31"/>
@@ -15230,7 +15224,7 @@
       <c r="AC204" s="31"/>
       <c r="AD204" s="31"/>
     </row>
-    <row r="205" spans="1:30">
+    <row r="205" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A205" s="31"/>
       <c r="B205" s="31"/>
       <c r="C205" s="31"/>
@@ -15280,7 +15274,7 @@
       <c r="AC205" s="31"/>
       <c r="AD205" s="31"/>
     </row>
-    <row r="206" spans="1:30">
+    <row r="206" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A206" s="31"/>
       <c r="B206" s="31"/>
       <c r="C206" s="31"/>
@@ -15330,7 +15324,7 @@
       <c r="AC206" s="31"/>
       <c r="AD206" s="31"/>
     </row>
-    <row r="207" spans="1:30">
+    <row r="207" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A207" s="31"/>
       <c r="B207" s="31"/>
       <c r="C207" s="31"/>
@@ -15380,7 +15374,7 @@
       <c r="AC207" s="31"/>
       <c r="AD207" s="31"/>
     </row>
-    <row r="208" spans="1:30">
+    <row r="208" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A208" s="31"/>
       <c r="B208" s="31"/>
       <c r="C208" s="31"/>
@@ -15430,7 +15424,7 @@
       <c r="AC208" s="31"/>
       <c r="AD208" s="31"/>
     </row>
-    <row r="209" spans="1:30">
+    <row r="209" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A209" s="31"/>
       <c r="B209" s="31"/>
       <c r="C209" s="31"/>
@@ -15480,7 +15474,7 @@
       <c r="AC209" s="31"/>
       <c r="AD209" s="31"/>
     </row>
-    <row r="210" spans="1:30" ht="15">
+    <row r="210" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A210" s="31"/>
       <c r="B210" s="31"/>
       <c r="C210" s="31"/>
@@ -15528,7 +15522,7 @@
       <c r="AC210" s="31"/>
       <c r="AD210" s="31"/>
     </row>
-    <row r="211" spans="1:30">
+    <row r="211" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A211" s="31"/>
       <c r="B211" s="31"/>
       <c r="C211" s="31"/>
@@ -15576,7 +15570,7 @@
       <c r="AC211" s="31"/>
       <c r="AD211" s="31"/>
     </row>
-    <row r="212" spans="1:30">
+    <row r="212" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A212" s="31"/>
       <c r="B212" s="31"/>
       <c r="C212" s="31"/>
@@ -15624,7 +15618,7 @@
       <c r="AC212" s="31"/>
       <c r="AD212" s="31"/>
     </row>
-    <row r="213" spans="1:30">
+    <row r="213" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A213" s="31"/>
       <c r="B213" s="31"/>
       <c r="C213" s="31"/>
@@ -15674,7 +15668,7 @@
       <c r="AC213" s="31"/>
       <c r="AD213" s="31"/>
     </row>
-    <row r="214" spans="1:30">
+    <row r="214" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A214" s="31"/>
       <c r="B214" s="31"/>
       <c r="C214" s="31"/>
@@ -15728,7 +15722,7 @@
       <c r="AC214" s="31"/>
       <c r="AD214" s="31"/>
     </row>
-    <row r="215" spans="1:30" ht="15">
+    <row r="215" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A215" s="31"/>
       <c r="B215" s="31"/>
       <c r="C215" s="31"/>
@@ -15778,7 +15772,7 @@
       <c r="AC215" s="31"/>
       <c r="AD215" s="31"/>
     </row>
-    <row r="216" spans="1:30" ht="15">
+    <row r="216" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A216" s="31"/>
       <c r="B216" s="31"/>
       <c r="C216" s="31"/>
@@ -15828,7 +15822,7 @@
       <c r="AC216" s="31"/>
       <c r="AD216" s="31"/>
     </row>
-    <row r="217" spans="1:30">
+    <row r="217" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A217" s="31"/>
       <c r="B217" s="31"/>
       <c r="C217" s="31"/>
@@ -15878,7 +15872,7 @@
       <c r="AC217" s="31"/>
       <c r="AD217" s="31"/>
     </row>
-    <row r="218" spans="1:30">
+    <row r="218" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A218" s="31"/>
       <c r="B218" s="31"/>
       <c r="C218" s="31"/>
@@ -15928,7 +15922,7 @@
       <c r="AC218" s="31"/>
       <c r="AD218" s="31"/>
     </row>
-    <row r="219" spans="1:30">
+    <row r="219" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A219" s="31"/>
       <c r="B219" s="31"/>
       <c r="C219" s="31"/>
@@ -15978,7 +15972,7 @@
       <c r="AC219" s="31"/>
       <c r="AD219" s="31"/>
     </row>
-    <row r="220" spans="1:30" ht="15">
+    <row r="220" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A220" s="31"/>
       <c r="B220" s="31"/>
       <c r="C220" s="31"/>
@@ -16028,7 +16022,7 @@
       <c r="AC220" s="31"/>
       <c r="AD220" s="31"/>
     </row>
-    <row r="221" spans="1:30">
+    <row r="221" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A221" s="31"/>
       <c r="B221" s="31"/>
       <c r="C221" s="31"/>
@@ -16078,7 +16072,7 @@
       <c r="AC221" s="31"/>
       <c r="AD221" s="31"/>
     </row>
-    <row r="222" spans="1:30">
+    <row r="222" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A222" s="31"/>
       <c r="B222" s="31"/>
       <c r="C222" s="31"/>
@@ -16128,7 +16122,7 @@
       <c r="AC222" s="31"/>
       <c r="AD222" s="31"/>
     </row>
-    <row r="223" spans="1:30">
+    <row r="223" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A223" s="31"/>
       <c r="B223" s="31"/>
       <c r="C223" s="31"/>
@@ -16176,7 +16170,7 @@
       <c r="AC223" s="31"/>
       <c r="AD223" s="31"/>
     </row>
-    <row r="224" spans="1:30">
+    <row r="224" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A224" s="31"/>
       <c r="B224" s="31"/>
       <c r="C224" s="31"/>
@@ -16224,7 +16218,7 @@
       <c r="AC224" s="31"/>
       <c r="AD224" s="31"/>
     </row>
-    <row r="225" spans="1:30">
+    <row r="225" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A225" s="31"/>
       <c r="B225" s="31"/>
       <c r="C225" s="31"/>
@@ -16272,7 +16266,7 @@
       <c r="AC225" s="31"/>
       <c r="AD225" s="31"/>
     </row>
-    <row r="226" spans="1:30">
+    <row r="226" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A226" s="31"/>
       <c r="B226" s="31"/>
       <c r="C226" s="31"/>
@@ -16322,7 +16316,7 @@
       <c r="AC226" s="31"/>
       <c r="AD226" s="31"/>
     </row>
-    <row r="227" spans="1:30">
+    <row r="227" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A227" s="31"/>
       <c r="B227" s="31"/>
       <c r="C227" s="31"/>
@@ -16372,7 +16366,7 @@
       <c r="AC227" s="31"/>
       <c r="AD227" s="31"/>
     </row>
-    <row r="228" spans="1:30">
+    <row r="228" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A228" s="31"/>
       <c r="B228" s="31"/>
       <c r="C228" s="31"/>
@@ -16422,7 +16416,7 @@
       <c r="AC228" s="31"/>
       <c r="AD228" s="31"/>
     </row>
-    <row r="229" spans="1:30" ht="15">
+    <row r="229" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A229" s="31"/>
       <c r="B229" s="31"/>
       <c r="C229" s="31"/>
@@ -16472,7 +16466,7 @@
       <c r="AC229" s="31"/>
       <c r="AD229" s="31"/>
     </row>
-    <row r="230" spans="1:30">
+    <row r="230" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A230" s="31"/>
       <c r="B230" s="31"/>
       <c r="C230" s="31"/>
@@ -16522,7 +16516,7 @@
       <c r="AC230" s="31"/>
       <c r="AD230" s="31"/>
     </row>
-    <row r="231" spans="1:30">
+    <row r="231" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A231" s="31"/>
       <c r="B231" s="31"/>
       <c r="C231" s="31"/>
@@ -16572,7 +16566,7 @@
       <c r="AC231" s="31"/>
       <c r="AD231" s="31"/>
     </row>
-    <row r="232" spans="1:30" ht="15">
+    <row r="232" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A232" s="31"/>
       <c r="B232" s="31"/>
       <c r="C232" s="31"/>
@@ -16622,7 +16616,7 @@
       <c r="AC232" s="31"/>
       <c r="AD232" s="31"/>
     </row>
-    <row r="233" spans="1:30" ht="15">
+    <row r="233" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A233" s="31"/>
       <c r="B233" s="31"/>
       <c r="C233" s="31"/>
@@ -16670,7 +16664,7 @@
       <c r="AC233" s="31"/>
       <c r="AD233" s="31"/>
     </row>
-    <row r="234" spans="1:30">
+    <row r="234" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A234" s="31"/>
       <c r="B234" s="31"/>
       <c r="C234" s="31"/>
@@ -16718,7 +16712,7 @@
       <c r="AC234" s="31"/>
       <c r="AD234" s="31"/>
     </row>
-    <row r="235" spans="1:30">
+    <row r="235" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A235" s="31"/>
       <c r="B235" s="31"/>
       <c r="C235" s="31"/>
@@ -16766,7 +16760,7 @@
       <c r="AC235" s="31"/>
       <c r="AD235" s="31"/>
     </row>
-    <row r="236" spans="1:30">
+    <row r="236" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A236" s="31"/>
       <c r="B236" s="31"/>
       <c r="C236" s="31"/>
@@ -16814,7 +16808,7 @@
       <c r="AC236" s="31"/>
       <c r="AD236" s="31"/>
     </row>
-    <row r="237" spans="1:30">
+    <row r="237" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A237" s="31"/>
       <c r="B237" s="31"/>
       <c r="C237" s="31"/>
@@ -16864,7 +16858,7 @@
       <c r="AC237" s="31"/>
       <c r="AD237" s="31"/>
     </row>
-    <row r="238" spans="1:30">
+    <row r="238" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A238" s="31"/>
       <c r="B238" s="31"/>
       <c r="C238" s="31"/>
@@ -16914,7 +16908,7 @@
       <c r="AC238" s="31"/>
       <c r="AD238" s="31"/>
     </row>
-    <row r="239" spans="1:30" ht="15">
+    <row r="239" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A239" s="31"/>
       <c r="B239" s="31"/>
       <c r="C239" s="31"/>
@@ -16964,7 +16958,7 @@
       <c r="AC239" s="31"/>
       <c r="AD239" s="31"/>
     </row>
-    <row r="240" spans="1:30">
+    <row r="240" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A240" s="31"/>
       <c r="B240" s="31"/>
       <c r="C240" s="31"/>
@@ -17014,7 +17008,7 @@
       <c r="AC240" s="31"/>
       <c r="AD240" s="31"/>
     </row>
-    <row r="241" spans="1:30">
+    <row r="241" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A241" s="31"/>
       <c r="B241" s="31"/>
       <c r="C241" s="31"/>
@@ -17064,7 +17058,7 @@
       <c r="AC241" s="31"/>
       <c r="AD241" s="31"/>
     </row>
-    <row r="242" spans="1:30">
+    <row r="242" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A242" s="31"/>
       <c r="B242" s="31"/>
       <c r="C242" s="31"/>
@@ -17112,7 +17106,7 @@
       <c r="AC242" s="31"/>
       <c r="AD242" s="31"/>
     </row>
-    <row r="243" spans="1:30">
+    <row r="243" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A243" s="31"/>
       <c r="B243" s="31"/>
       <c r="C243" s="31"/>
@@ -17160,7 +17154,7 @@
       <c r="AC243" s="31"/>
       <c r="AD243" s="31"/>
     </row>
-    <row r="244" spans="1:30">
+    <row r="244" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A244" s="31"/>
       <c r="B244" s="31"/>
       <c r="C244" s="31"/>
@@ -17208,7 +17202,7 @@
       <c r="AC244" s="31"/>
       <c r="AD244" s="31"/>
     </row>
-    <row r="245" spans="1:30">
+    <row r="245" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A245" s="31"/>
       <c r="B245" s="31"/>
       <c r="C245" s="31"/>
@@ -17256,7 +17250,7 @@
       <c r="AC245" s="31"/>
       <c r="AD245" s="31"/>
     </row>
-    <row r="246" spans="1:30">
+    <row r="246" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A246" s="31"/>
       <c r="B246" s="31"/>
       <c r="C246" s="31"/>
@@ -17304,7 +17298,7 @@
       <c r="AC246" s="31"/>
       <c r="AD246" s="31"/>
     </row>
-    <row r="247" spans="1:30" ht="15">
+    <row r="247" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A247" s="31"/>
       <c r="B247" s="31"/>
       <c r="C247" s="31"/>
@@ -17352,7 +17346,7 @@
       <c r="AC247" s="31"/>
       <c r="AD247" s="31"/>
     </row>
-    <row r="248" spans="1:30" ht="15">
+    <row r="248" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A248" s="31"/>
       <c r="B248" s="31"/>
       <c r="C248" s="31"/>
@@ -17402,7 +17396,7 @@
       <c r="AC248" s="31"/>
       <c r="AD248" s="31"/>
     </row>
-    <row r="249" spans="1:30">
+    <row r="249" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A249" s="31"/>
       <c r="B249" s="31"/>
       <c r="C249" s="31"/>
@@ -17452,7 +17446,7 @@
       <c r="AC249" s="31"/>
       <c r="AD249" s="31"/>
     </row>
-    <row r="250" spans="1:30">
+    <row r="250" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A250" s="31"/>
       <c r="B250" s="31"/>
       <c r="C250" s="31"/>
@@ -17502,7 +17496,7 @@
       <c r="AC250" s="31"/>
       <c r="AD250" s="31"/>
     </row>
-    <row r="251" spans="1:30">
+    <row r="251" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A251" s="31"/>
       <c r="B251" s="31"/>
       <c r="C251" s="31"/>
@@ -17552,7 +17546,7 @@
       <c r="AC251" s="31"/>
       <c r="AD251" s="31"/>
     </row>
-    <row r="252" spans="1:30" ht="15">
+    <row r="252" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A252" s="31"/>
       <c r="B252" s="31"/>
       <c r="C252" s="31"/>
@@ -17600,7 +17594,7 @@
       <c r="AC252" s="31"/>
       <c r="AD252" s="31"/>
     </row>
-    <row r="253" spans="1:30">
+    <row r="253" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A253" s="31"/>
       <c r="B253" s="31"/>
       <c r="C253" s="31"/>
@@ -17648,7 +17642,7 @@
       <c r="AC253" s="31"/>
       <c r="AD253" s="31"/>
     </row>
-    <row r="254" spans="1:30">
+    <row r="254" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A254" s="31"/>
       <c r="B254" s="31"/>
       <c r="C254" s="31"/>
@@ -17696,7 +17690,7 @@
       <c r="AC254" s="31"/>
       <c r="AD254" s="31"/>
     </row>
-    <row r="255" spans="1:30">
+    <row r="255" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A255" s="31"/>
       <c r="B255" s="31"/>
       <c r="C255" s="31"/>
@@ -17750,7 +17744,7 @@
       </c>
       <c r="AD255" s="31"/>
     </row>
-    <row r="256" spans="1:30" ht="15">
+    <row r="256" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A256" s="31"/>
       <c r="B256" s="31"/>
       <c r="C256" s="31"/>
@@ -17796,7 +17790,7 @@
       <c r="AC256" s="31"/>
       <c r="AD256" s="31"/>
     </row>
-    <row r="257" spans="1:30">
+    <row r="257" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A257" s="31"/>
       <c r="B257" s="31"/>
       <c r="C257" s="31"/>
@@ -17842,7 +17836,7 @@
       <c r="AC257" s="31"/>
       <c r="AD257" s="31"/>
     </row>
-    <row r="258" spans="1:30" ht="15">
+    <row r="258" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A258" s="31"/>
       <c r="B258" s="31"/>
       <c r="C258" s="31"/>
@@ -17892,7 +17886,7 @@
       <c r="AC258" s="31"/>
       <c r="AD258" s="31"/>
     </row>
-    <row r="259" spans="1:30" ht="15">
+    <row r="259" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A259" s="31"/>
       <c r="B259" s="31"/>
       <c r="D259" s="38"/>
@@ -17939,7 +17933,7 @@
       <c r="AC259" s="31"/>
       <c r="AD259" s="31"/>
     </row>
-    <row r="260" spans="1:30" ht="15">
+    <row r="260" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A260" s="31"/>
       <c r="B260" s="31"/>
       <c r="D260" s="38"/>
@@ -17988,7 +17982,7 @@
       <c r="AC260" s="31"/>
       <c r="AD260" s="31"/>
     </row>
-    <row r="261" spans="1:30" ht="15">
+    <row r="261" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A261" s="31"/>
       <c r="B261" s="31"/>
       <c r="C261" s="31" t="s">
@@ -18052,7 +18046,7 @@
       <c r="AC261" s="31"/>
       <c r="AD261" s="31"/>
     </row>
-    <row r="262" spans="1:30" ht="15">
+    <row r="262" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A262" s="31"/>
       <c r="B262" s="31"/>
       <c r="C262" s="31" t="s">
@@ -18116,7 +18110,7 @@
       <c r="AC262" s="31"/>
       <c r="AD262" s="31"/>
     </row>
-    <row r="263" spans="1:30" ht="15">
+    <row r="263" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A263" s="31"/>
       <c r="B263" s="31"/>
       <c r="C263" s="31" t="s">
@@ -18178,7 +18172,7 @@
       <c r="AC263" s="31"/>
       <c r="AD263" s="31"/>
     </row>
-    <row r="264" spans="1:30" ht="15">
+    <row r="264" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A264" s="31"/>
       <c r="B264" s="31"/>
       <c r="C264" s="31" t="s">
@@ -18236,7 +18230,7 @@
       <c r="AC264" s="31"/>
       <c r="AD264" s="31"/>
     </row>
-    <row r="265" spans="1:30" ht="15">
+    <row r="265" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A265" s="31"/>
       <c r="B265" s="31"/>
       <c r="C265" s="31"/>
@@ -18284,7 +18278,7 @@
       <c r="AC265" s="31"/>
       <c r="AD265" s="31"/>
     </row>
-    <row r="266" spans="1:30">
+    <row r="266" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A266" s="31"/>
       <c r="B266" s="31"/>
       <c r="C266" s="31"/>
@@ -18332,7 +18326,7 @@
       <c r="AC266" s="31"/>
       <c r="AD266" s="31"/>
     </row>
-    <row r="267" spans="1:30">
+    <row r="267" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A267" s="31"/>
       <c r="B267" s="31"/>
       <c r="C267" s="31" t="s">
@@ -18390,7 +18384,7 @@
       <c r="AC267" s="31"/>
       <c r="AD267" s="31"/>
     </row>
-    <row r="268" spans="1:30">
+    <row r="268" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A268" s="31"/>
       <c r="B268" s="31"/>
       <c r="C268" s="31" t="s">
@@ -18440,7 +18434,7 @@
       <c r="AC268" s="31"/>
       <c r="AD268" s="31"/>
     </row>
-    <row r="269" spans="1:30" ht="15">
+    <row r="269" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A269" s="31"/>
       <c r="B269" s="31"/>
       <c r="C269" s="31"/>
@@ -18490,7 +18484,7 @@
       <c r="AC269" s="31"/>
       <c r="AD269" s="31"/>
     </row>
-    <row r="270" spans="1:30" ht="15">
+    <row r="270" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A270" s="31"/>
       <c r="B270" s="31"/>
       <c r="C270" s="31" t="s">
@@ -18550,7 +18544,7 @@
       <c r="AC270" s="31"/>
       <c r="AD270" s="31"/>
     </row>
-    <row r="271" spans="1:30" ht="15">
+    <row r="271" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A271" s="31"/>
       <c r="B271" s="31"/>
       <c r="C271" s="31" t="s">
@@ -18614,7 +18608,7 @@
       <c r="AC271" s="31"/>
       <c r="AD271" s="31"/>
     </row>
-    <row r="272" spans="1:30">
+    <row r="272" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A272" s="31"/>
       <c r="B272" s="31"/>
       <c r="C272" s="31"/>
@@ -18666,7 +18660,7 @@
       <c r="AC272" s="31"/>
       <c r="AD272" s="31"/>
     </row>
-    <row r="273" spans="1:30" ht="15">
+    <row r="273" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A273" s="31"/>
       <c r="B273" s="31"/>
       <c r="C273" s="31"/>
@@ -18716,7 +18710,7 @@
       <c r="AC273" s="31"/>
       <c r="AD273" s="31"/>
     </row>
-    <row r="274" spans="1:30" ht="15">
+    <row r="274" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A274" s="31"/>
       <c r="B274" s="31"/>
       <c r="C274" s="31" t="s">
@@ -18782,7 +18776,7 @@
       <c r="AC274" s="31"/>
       <c r="AD274" s="31"/>
     </row>
-    <row r="275" spans="1:30" ht="15">
+    <row r="275" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A275" s="31"/>
       <c r="B275" s="31"/>
       <c r="C275" s="31" t="s">
@@ -18844,7 +18838,7 @@
       <c r="AC275" s="31"/>
       <c r="AD275" s="31"/>
     </row>
-    <row r="276" spans="1:30" ht="15">
+    <row r="276" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A276" s="31"/>
       <c r="B276" s="31"/>
       <c r="C276" s="31"/>
@@ -18898,7 +18892,7 @@
       <c r="AC276" s="31"/>
       <c r="AD276" s="31"/>
     </row>
-    <row r="277" spans="1:30" ht="15">
+    <row r="277" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A277" s="31"/>
       <c r="B277" s="31"/>
       <c r="C277" s="31" t="s">
@@ -18956,7 +18950,7 @@
       <c r="AC277" s="31"/>
       <c r="AD277" s="31"/>
     </row>
-    <row r="278" spans="1:30" ht="15">
+    <row r="278" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A278" s="31"/>
       <c r="B278" s="31"/>
       <c r="C278" s="31" t="s">
@@ -19018,7 +19012,7 @@
       <c r="AC278" s="31"/>
       <c r="AD278" s="31"/>
     </row>
-    <row r="279" spans="1:30" ht="15">
+    <row r="279" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A279" s="31"/>
       <c r="B279" s="31"/>
       <c r="C279" s="31" t="s">
@@ -19070,7 +19064,7 @@
       <c r="AC279" s="31"/>
       <c r="AD279" s="31"/>
     </row>
-    <row r="280" spans="1:30" ht="15">
+    <row r="280" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A280" s="31"/>
       <c r="B280" s="31"/>
       <c r="C280" s="31" t="s">
@@ -19120,7 +19114,7 @@
       <c r="AC280" s="31"/>
       <c r="AD280" s="31"/>
     </row>
-    <row r="281" spans="1:30" ht="15">
+    <row r="281" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A281" s="31"/>
       <c r="B281" s="31"/>
       <c r="C281" s="31" t="s">
@@ -19170,7 +19164,7 @@
       <c r="AC281" s="31"/>
       <c r="AD281" s="31"/>
     </row>
-    <row r="282" spans="1:30">
+    <row r="282" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A282" s="31"/>
       <c r="B282" s="31"/>
       <c r="C282" s="31"/>
@@ -19224,7 +19218,7 @@
       <c r="AC282" s="31"/>
       <c r="AD282" s="31"/>
     </row>
-    <row r="283" spans="1:30" ht="15">
+    <row r="283" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A283" s="31"/>
       <c r="B283" s="31"/>
       <c r="C283" s="31" t="s">
@@ -19290,7 +19284,7 @@
       <c r="AC283" s="31"/>
       <c r="AD283" s="31"/>
     </row>
-    <row r="284" spans="1:30">
+    <row r="284" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A284" s="31"/>
       <c r="B284" s="31"/>
       <c r="C284" s="31"/>
@@ -19342,7 +19336,7 @@
       <c r="AC284" s="31"/>
       <c r="AD284" s="31"/>
     </row>
-    <row r="285" spans="1:30">
+    <row r="285" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A285" s="31"/>
       <c r="B285" s="31"/>
       <c r="C285" s="31"/>
@@ -19404,7 +19398,7 @@
       </c>
       <c r="AD285" s="31"/>
     </row>
-    <row r="286" spans="1:30" ht="15">
+    <row r="286" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A286" s="31"/>
       <c r="B286" s="31"/>
       <c r="C286" s="31"/>
@@ -19450,7 +19444,7 @@
       <c r="AC286" s="31"/>
       <c r="AD286" s="31"/>
     </row>
-    <row r="287" spans="1:30">
+    <row r="287" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A287" s="31"/>
       <c r="B287" s="31"/>
       <c r="C287" s="31"/>
@@ -19502,7 +19496,7 @@
       <c r="AC287" s="31"/>
       <c r="AD287" s="31"/>
     </row>
-    <row r="288" spans="1:30">
+    <row r="288" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A288" s="31"/>
       <c r="B288" s="31" t="s">
         <v>150</v>
@@ -19564,7 +19558,7 @@
       <c r="AC288" s="31"/>
       <c r="AD288" s="31"/>
     </row>
-    <row r="289" spans="1:30">
+    <row r="289" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A289" s="31"/>
       <c r="B289" s="31"/>
       <c r="C289" s="31"/>
@@ -19612,7 +19606,7 @@
       <c r="AC289" s="31"/>
       <c r="AD289" s="31"/>
     </row>
-    <row r="290" spans="1:30">
+    <row r="290" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A290" s="31"/>
       <c r="B290" s="31"/>
       <c r="C290" s="31"/>
@@ -19660,7 +19654,7 @@
       <c r="AC290" s="31"/>
       <c r="AD290" s="31"/>
     </row>
-    <row r="291" spans="1:30">
+    <row r="291" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A291" s="31"/>
       <c r="B291" s="31"/>
       <c r="C291" s="31"/>
@@ -19708,7 +19702,7 @@
       <c r="AC291" s="31"/>
       <c r="AD291" s="31"/>
     </row>
-    <row r="292" spans="1:30">
+    <row r="292" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A292" s="31"/>
       <c r="B292" s="31"/>
       <c r="C292" s="31"/>
@@ -19762,7 +19756,7 @@
       <c r="AC292" s="31"/>
       <c r="AD292" s="31"/>
     </row>
-    <row r="293" spans="1:30">
+    <row r="293" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A293" s="31"/>
       <c r="B293" s="31"/>
       <c r="C293" s="31"/>
@@ -19814,7 +19808,7 @@
       <c r="AC293" s="31"/>
       <c r="AD293" s="31"/>
     </row>
-    <row r="294" spans="1:30">
+    <row r="294" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A294" s="31"/>
       <c r="B294" s="31"/>
       <c r="C294" s="31"/>
@@ -19866,7 +19860,7 @@
       <c r="AC294" s="31"/>
       <c r="AD294" s="31"/>
     </row>
-    <row r="295" spans="1:30">
+    <row r="295" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A295" s="31"/>
       <c r="B295" s="31"/>
       <c r="C295" s="31"/>
@@ -19918,7 +19912,7 @@
       <c r="AC295" s="31"/>
       <c r="AD295" s="31"/>
     </row>
-    <row r="296" spans="1:30">
+    <row r="296" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A296" s="31"/>
       <c r="B296" s="31"/>
       <c r="C296" s="31"/>
@@ -19970,7 +19964,7 @@
       <c r="AC296" s="31"/>
       <c r="AD296" s="31"/>
     </row>
-    <row r="297" spans="1:30">
+    <row r="297" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A297" s="31"/>
       <c r="B297" s="31"/>
       <c r="C297" s="31"/>
@@ -20024,7 +20018,7 @@
       <c r="AC297" s="31"/>
       <c r="AD297" s="31"/>
     </row>
-    <row r="298" spans="1:30" ht="15">
+    <row r="298" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A298" s="31"/>
       <c r="B298" s="31"/>
       <c r="C298" s="31"/>
@@ -20070,7 +20064,7 @@
       <c r="AC298" s="31"/>
       <c r="AD298" s="31"/>
     </row>
-    <row r="299" spans="1:30">
+    <row r="299" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A299" s="31"/>
       <c r="B299" s="31"/>
       <c r="C299" s="31"/>
@@ -20120,7 +20114,7 @@
       <c r="AC299" s="31"/>
       <c r="AD299" s="31"/>
     </row>
-    <row r="300" spans="1:30">
+    <row r="300" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A300" s="31"/>
       <c r="B300" s="31"/>
       <c r="C300" s="31"/>
@@ -20172,7 +20166,7 @@
       <c r="AC300" s="31"/>
       <c r="AD300" s="31"/>
     </row>
-    <row r="301" spans="1:30" ht="15">
+    <row r="301" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A301" s="31"/>
       <c r="B301" s="31"/>
       <c r="C301" s="31"/>
@@ -20226,7 +20220,7 @@
       <c r="AC301" s="31"/>
       <c r="AD301" s="31"/>
     </row>
-    <row r="302" spans="1:30" ht="15">
+    <row r="302" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A302" s="31"/>
       <c r="B302" s="31"/>
       <c r="C302" s="31"/>
@@ -20274,7 +20268,7 @@
       <c r="AC302" s="31"/>
       <c r="AD302" s="31"/>
     </row>
-    <row r="303" spans="1:30">
+    <row r="303" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A303" s="31"/>
       <c r="B303" s="31"/>
       <c r="C303" s="31"/>
@@ -20322,7 +20316,7 @@
       <c r="AC303" s="31"/>
       <c r="AD303" s="31"/>
     </row>
-    <row r="304" spans="1:30">
+    <row r="304" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A304" s="31"/>
       <c r="B304" s="31"/>
       <c r="C304" s="31"/>
@@ -20370,7 +20364,7 @@
       <c r="AC304" s="31"/>
       <c r="AD304" s="31"/>
     </row>
-    <row r="305" spans="1:30">
+    <row r="305" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A305" s="31"/>
       <c r="B305" s="31"/>
       <c r="C305" s="31"/>
@@ -20424,7 +20418,7 @@
       <c r="AC305" s="31"/>
       <c r="AD305" s="31"/>
     </row>
-    <row r="306" spans="1:30">
+    <row r="306" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A306" s="31"/>
       <c r="B306" s="31"/>
       <c r="C306" s="31"/>
@@ -20474,7 +20468,7 @@
       <c r="AC306" s="31"/>
       <c r="AD306" s="31"/>
     </row>
-    <row r="307" spans="1:30">
+    <row r="307" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A307" s="31"/>
       <c r="B307" s="31"/>
       <c r="C307" s="31"/>
@@ -20522,7 +20516,7 @@
       <c r="AC307" s="31"/>
       <c r="AD307" s="31"/>
     </row>
-    <row r="308" spans="1:30">
+    <row r="308" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A308" s="34"/>
       <c r="B308" s="34"/>
       <c r="C308" s="34" t="s">
@@ -20584,7 +20578,7 @@
       <c r="AC308" s="31"/>
       <c r="AD308" s="31"/>
     </row>
-    <row r="309" spans="1:30">
+    <row r="309" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A309" s="34"/>
       <c r="B309" s="34"/>
       <c r="C309" s="34" t="s">
@@ -20648,7 +20642,7 @@
       <c r="AC309" s="31"/>
       <c r="AD309" s="31"/>
     </row>
-    <row r="310" spans="1:30">
+    <row r="310" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A310" s="31"/>
       <c r="B310" s="31"/>
       <c r="C310" s="31"/>
@@ -20700,7 +20694,7 @@
       <c r="AC310" s="31"/>
       <c r="AD310" s="31"/>
     </row>
-    <row r="311" spans="1:30">
+    <row r="311" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A311" s="34"/>
       <c r="B311" s="34"/>
       <c r="C311" s="34" t="s">
@@ -20764,7 +20758,7 @@
       <c r="AC311" s="31"/>
       <c r="AD311" s="31"/>
     </row>
-    <row r="312" spans="1:30">
+    <row r="312" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A312" s="34"/>
       <c r="B312" s="34"/>
       <c r="C312" s="34" t="s">
@@ -20818,7 +20812,7 @@
       <c r="AC312" s="31"/>
       <c r="AD312" s="31"/>
     </row>
-    <row r="313" spans="1:30">
+    <row r="313" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A313" s="31"/>
       <c r="B313" s="31"/>
       <c r="C313" s="31"/>
@@ -20866,7 +20860,7 @@
       <c r="AC313" s="31"/>
       <c r="AD313" s="31"/>
     </row>
-    <row r="314" spans="1:30" ht="15">
+    <row r="314" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A314" s="34"/>
       <c r="B314" s="34"/>
       <c r="C314" s="34" t="s">
@@ -20928,7 +20922,7 @@
       <c r="AC314" s="31"/>
       <c r="AD314" s="31"/>
     </row>
-    <row r="315" spans="1:30" ht="15">
+    <row r="315" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A315" s="34"/>
       <c r="B315" s="34"/>
       <c r="C315" s="34" t="s">
@@ -20990,7 +20984,7 @@
       <c r="AC315" s="31"/>
       <c r="AD315" s="31"/>
     </row>
-    <row r="316" spans="1:30">
+    <row r="316" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A316" s="34"/>
       <c r="B316" s="34"/>
       <c r="C316" s="34" t="s">
@@ -21056,7 +21050,7 @@
       <c r="AC316" s="31"/>
       <c r="AD316" s="31"/>
     </row>
-    <row r="317" spans="1:30">
+    <row r="317" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A317" s="34"/>
       <c r="B317" s="34"/>
       <c r="C317" s="34" t="s">
@@ -21120,7 +21114,7 @@
       <c r="AC317" s="31"/>
       <c r="AD317" s="31"/>
     </row>
-    <row r="318" spans="1:30" ht="15">
+    <row r="318" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A318" s="31"/>
       <c r="B318" s="31"/>
       <c r="C318" s="31"/>
@@ -21168,7 +21162,7 @@
       <c r="AC318" s="31"/>
       <c r="AD318" s="31"/>
     </row>
-    <row r="319" spans="1:30">
+    <row r="319" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A319" s="31"/>
       <c r="B319" s="31"/>
       <c r="C319" s="31"/>
@@ -21214,7 +21208,7 @@
       <c r="AC319" s="31"/>
       <c r="AD319" s="31"/>
     </row>
-    <row r="320" spans="1:30">
+    <row r="320" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A320" s="31"/>
       <c r="B320" s="31"/>
       <c r="C320" s="31"/>
@@ -21258,7 +21252,7 @@
       <c r="AC320" s="31"/>
       <c r="AD320" s="31"/>
     </row>
-    <row r="321" spans="1:30">
+    <row r="321" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A321" s="31"/>
       <c r="B321" s="31"/>
       <c r="C321" s="31"/>
@@ -21311,7 +21305,7 @@
       <c r="AC321" s="31"/>
       <c r="AD321" s="31"/>
     </row>
-    <row r="322" spans="1:30">
+    <row r="322" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A322" s="32"/>
       <c r="B322" s="32"/>
       <c r="C322" s="32"/>
@@ -21353,7 +21347,7 @@
       <c r="AC322" s="31"/>
       <c r="AD322" s="31"/>
     </row>
-    <row r="323" spans="1:30">
+    <row r="323" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A323" s="31"/>
       <c r="B323" s="31"/>
       <c r="C323" s="31"/>
@@ -21407,7 +21401,7 @@
       <c r="AC323" s="31"/>
       <c r="AD323" s="31"/>
     </row>
-    <row r="324" spans="1:30" ht="15">
+    <row r="324" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A324" s="31"/>
       <c r="B324" s="31"/>
       <c r="C324" s="31"/>
@@ -21451,7 +21445,7 @@
       <c r="AC324" s="31"/>
       <c r="AD324" s="31"/>
     </row>
-    <row r="325" spans="1:30" ht="15">
+    <row r="325" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A325" s="31"/>
       <c r="B325" s="31"/>
       <c r="C325" s="31"/>
@@ -21495,7 +21489,7 @@
       <c r="AC325" s="31"/>
       <c r="AD325" s="31"/>
     </row>
-    <row r="326" spans="1:30" ht="15">
+    <row r="326" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A326" s="31"/>
       <c r="B326" s="31"/>
       <c r="C326" s="31"/>
@@ -21541,7 +21535,7 @@
       <c r="AC326" s="31"/>
       <c r="AD326" s="31"/>
     </row>
-    <row r="327" spans="1:30">
+    <row r="327" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L327" s="41" t="s">
         <v>790</v>
       </c>
@@ -21564,7 +21558,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="328" spans="1:30">
+    <row r="328" spans="1:30" x14ac:dyDescent="0.2">
       <c r="I328" s="37" t="s">
         <v>792</v>
       </c>
@@ -21587,7 +21581,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="329" spans="1:30" ht="15">
+    <row r="329" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A329" s="31"/>
       <c r="B329" s="31"/>
       <c r="C329" s="31"/>
@@ -21639,7 +21633,7 @@
       <c r="AC329" s="31"/>
       <c r="AD329" s="31"/>
     </row>
-    <row r="330" spans="1:30">
+    <row r="330" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A330" s="31"/>
       <c r="B330" s="31"/>
       <c r="C330" s="31"/>
@@ -21691,7 +21685,7 @@
       <c r="AC330" s="31"/>
       <c r="AD330" s="31"/>
     </row>
-    <row r="331" spans="1:30">
+    <row r="331" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A331" s="31"/>
       <c r="B331" s="31"/>
       <c r="C331" s="31"/>
@@ -21743,7 +21737,7 @@
       <c r="AC331" s="31"/>
       <c r="AD331" s="31"/>
     </row>
-    <row r="332" spans="1:30">
+    <row r="332" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A332" s="31"/>
       <c r="B332" s="31"/>
       <c r="C332" s="31"/>
@@ -21795,7 +21789,7 @@
       <c r="AC332" s="31"/>
       <c r="AD332" s="31"/>
     </row>
-    <row r="333" spans="1:30">
+    <row r="333" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A333" s="31"/>
       <c r="B333" s="31"/>
       <c r="C333" s="31"/>
@@ -21839,7 +21833,7 @@
       <c r="AC333" s="31"/>
       <c r="AD333" s="31"/>
     </row>
-    <row r="334" spans="1:30">
+    <row r="334" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A334" s="31"/>
       <c r="B334" s="31"/>
       <c r="C334" s="31"/>
@@ -21883,7 +21877,7 @@
       <c r="AC334" s="31"/>
       <c r="AD334" s="31"/>
     </row>
-    <row r="335" spans="1:30">
+    <row r="335" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A335" s="31" t="s">
         <v>147</v>
       </c>
@@ -21945,7 +21939,7 @@
       <c r="AC335" s="31"/>
       <c r="AD335" s="31"/>
     </row>
-    <row r="336" spans="1:30">
+    <row r="336" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A336" s="31"/>
       <c r="B336" s="31"/>
       <c r="C336" s="31"/>
@@ -21999,7 +21993,7 @@
       <c r="AC336" s="31"/>
       <c r="AD336" s="31"/>
     </row>
-    <row r="337" spans="1:30">
+    <row r="337" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A337" s="31"/>
       <c r="B337" s="31"/>
       <c r="C337" s="31"/>
@@ -22053,7 +22047,7 @@
       <c r="AC337" s="31"/>
       <c r="AD337" s="31"/>
     </row>
-    <row r="338" spans="1:30" ht="15">
+    <row r="338" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A338" s="31"/>
       <c r="B338" s="31"/>
       <c r="C338" s="31"/>
@@ -22101,7 +22095,7 @@
       <c r="AC338" s="31"/>
       <c r="AD338" s="31"/>
     </row>
-    <row r="339" spans="1:30" ht="15">
+    <row r="339" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A339" s="31"/>
       <c r="B339" s="31"/>
       <c r="C339" s="31"/>
@@ -22153,7 +22147,7 @@
       <c r="AC339" s="31"/>
       <c r="AD339" s="31"/>
     </row>
-    <row r="340" spans="1:30">
+    <row r="340" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A340" s="31"/>
       <c r="B340" s="31"/>
       <c r="C340" s="31"/>
@@ -22199,7 +22193,7 @@
       <c r="AC340" s="31"/>
       <c r="AD340" s="31"/>
     </row>
-    <row r="341" spans="1:30">
+    <row r="341" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A341" s="31"/>
       <c r="B341" s="31"/>
       <c r="C341" s="31"/>
@@ -22245,7 +22239,7 @@
       <c r="AC341" s="31"/>
       <c r="AD341" s="31"/>
     </row>
-    <row r="342" spans="1:30">
+    <row r="342" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A342" s="31"/>
       <c r="B342" s="31"/>
       <c r="C342" s="31"/>
@@ -22291,7 +22285,7 @@
       <c r="AC342" s="31"/>
       <c r="AD342" s="31"/>
     </row>
-    <row r="343" spans="1:30">
+    <row r="343" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A343" s="31"/>
       <c r="B343" s="31"/>
       <c r="C343" s="31"/>
@@ -22343,7 +22337,7 @@
       <c r="AC343" s="31"/>
       <c r="AD343" s="31"/>
     </row>
-    <row r="344" spans="1:30">
+    <row r="344" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A344" s="31"/>
       <c r="B344" s="31"/>
       <c r="C344" s="31"/>
@@ -22395,7 +22389,7 @@
       <c r="AC344" s="31"/>
       <c r="AD344" s="31"/>
     </row>
-    <row r="345" spans="1:30">
+    <row r="345" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A345" s="31"/>
       <c r="B345" s="31"/>
       <c r="C345" s="31"/>
@@ -22447,7 +22441,7 @@
       <c r="AC345" s="31"/>
       <c r="AD345" s="31"/>
     </row>
-    <row r="346" spans="1:30">
+    <row r="346" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A346" s="31"/>
       <c r="B346" s="31"/>
       <c r="C346" s="31"/>
@@ -22501,7 +22495,7 @@
       <c r="AC346" s="31"/>
       <c r="AD346" s="31"/>
     </row>
-    <row r="347" spans="1:30" ht="15">
+    <row r="347" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A347" s="31"/>
       <c r="B347" s="31"/>
       <c r="C347" s="31"/>
@@ -22553,7 +22547,7 @@
       <c r="AC347" s="31"/>
       <c r="AD347" s="31"/>
     </row>
-    <row r="348" spans="1:30" ht="15">
+    <row r="348" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A348" s="31"/>
       <c r="B348" s="31"/>
       <c r="C348" s="31"/>
@@ -22605,7 +22599,7 @@
       <c r="AC348" s="31"/>
       <c r="AD348" s="31"/>
     </row>
-    <row r="349" spans="1:30">
+    <row r="349" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A349" s="31"/>
       <c r="B349" s="31"/>
       <c r="C349" s="31"/>
@@ -22657,7 +22651,7 @@
       <c r="AC349" s="31"/>
       <c r="AD349" s="31"/>
     </row>
-    <row r="350" spans="1:30">
+    <row r="350" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A350" s="31"/>
       <c r="B350" s="31"/>
       <c r="C350" s="31"/>
@@ -22707,7 +22701,7 @@
       <c r="AC350" s="31"/>
       <c r="AD350" s="31"/>
     </row>
-    <row r="351" spans="1:30" ht="15">
+    <row r="351" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A351" s="31"/>
       <c r="B351" s="31"/>
       <c r="C351" s="31"/>
@@ -22761,7 +22755,7 @@
       <c r="AC351" s="31"/>
       <c r="AD351" s="31"/>
     </row>
-    <row r="352" spans="1:30">
+    <row r="352" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A352" s="31"/>
       <c r="B352" s="31"/>
       <c r="C352" s="31"/>
@@ -22811,7 +22805,7 @@
       <c r="AC352" s="31"/>
       <c r="AD352" s="31"/>
     </row>
-    <row r="353" spans="1:30">
+    <row r="353" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A353" s="31"/>
       <c r="B353" s="31"/>
       <c r="C353" s="31"/>
@@ -22859,7 +22853,7 @@
       <c r="AC353" s="31"/>
       <c r="AD353" s="31"/>
     </row>
-    <row r="354" spans="1:30" ht="15">
+    <row r="354" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A354" s="31"/>
       <c r="B354" s="31"/>
       <c r="C354" s="31"/>
@@ -22907,7 +22901,7 @@
       <c r="AC354" s="31"/>
       <c r="AD354" s="31"/>
     </row>
-    <row r="355" spans="1:30" ht="15">
+    <row r="355" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A355" s="31"/>
       <c r="B355" s="31"/>
       <c r="C355" s="31"/>
@@ -22951,7 +22945,7 @@
       <c r="AC355" s="31"/>
       <c r="AD355" s="31"/>
     </row>
-    <row r="356" spans="1:30" ht="15">
+    <row r="356" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A356" s="31"/>
       <c r="B356" s="31"/>
       <c r="C356" s="31"/>
@@ -22996,7 +22990,7 @@
       <c r="AC356" s="31"/>
       <c r="AD356" s="31"/>
     </row>
-    <row r="357" spans="1:30">
+    <row r="357" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A357" s="31"/>
       <c r="B357" s="31"/>
       <c r="C357" s="31"/>
@@ -23042,7 +23036,7 @@
       <c r="AC357" s="31"/>
       <c r="AD357" s="31"/>
     </row>
-    <row r="358" spans="1:30">
+    <row r="358" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A358" s="31"/>
       <c r="B358" s="31"/>
       <c r="C358" s="31"/>
@@ -23088,7 +23082,7 @@
       <c r="AC358" s="31"/>
       <c r="AD358" s="31"/>
     </row>
-    <row r="359" spans="1:30" ht="15">
+    <row r="359" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A359" s="31"/>
       <c r="B359" s="31"/>
       <c r="C359" s="31"/>
@@ -23132,7 +23126,7 @@
       <c r="AC359" s="31"/>
       <c r="AD359" s="31"/>
     </row>
-    <row r="360" spans="1:30">
+    <row r="360" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A360" s="31"/>
       <c r="B360" s="31"/>
       <c r="C360" s="31"/>
@@ -23184,7 +23178,7 @@
       <c r="AC360" s="31"/>
       <c r="AD360" s="31"/>
     </row>
-    <row r="361" spans="1:30">
+    <row r="361" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A361" s="31"/>
       <c r="B361" s="31"/>
       <c r="C361" s="31"/>
@@ -23228,7 +23222,7 @@
       <c r="AC361" s="31"/>
       <c r="AD361" s="31"/>
     </row>
-    <row r="362" spans="1:30" ht="15">
+    <row r="362" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A362" s="31"/>
       <c r="B362" s="31"/>
       <c r="C362" s="31"/>
@@ -23282,7 +23276,7 @@
       <c r="AC362" s="31"/>
       <c r="AD362" s="31"/>
     </row>
-    <row r="363" spans="1:30">
+    <row r="363" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A363" s="32" t="s">
         <v>126</v>
       </c>
@@ -23348,7 +23342,7 @@
       <c r="AC363" s="31"/>
       <c r="AD363" s="31"/>
     </row>
-    <row r="364" spans="1:30" ht="15">
+    <row r="364" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A364" s="31"/>
       <c r="B364" s="31"/>
       <c r="C364" s="31"/>
@@ -23400,7 +23394,7 @@
       <c r="AC364" s="31"/>
       <c r="AD364" s="31"/>
     </row>
-    <row r="365" spans="1:30" ht="15">
+    <row r="365" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A365" s="31"/>
       <c r="B365" s="31"/>
       <c r="C365" s="31"/>
@@ -23452,7 +23446,7 @@
       <c r="AC365" s="31"/>
       <c r="AD365" s="31"/>
     </row>
-    <row r="366" spans="1:30">
+    <row r="366" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A366" s="32" t="s">
         <v>129</v>
       </c>
@@ -23518,7 +23512,7 @@
       <c r="AC366" s="31"/>
       <c r="AD366" s="31"/>
     </row>
-    <row r="367" spans="1:30" ht="15">
+    <row r="367" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A367" s="31"/>
       <c r="B367" s="31"/>
       <c r="C367" s="31"/>
@@ -23570,7 +23564,7 @@
       <c r="AC367" s="31"/>
       <c r="AD367" s="31"/>
     </row>
-    <row r="368" spans="1:30">
+    <row r="368" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A368" s="32" t="s">
         <v>136</v>
       </c>
@@ -23636,7 +23630,7 @@
       <c r="AC368" s="31"/>
       <c r="AD368" s="31"/>
     </row>
-    <row r="369" spans="1:30">
+    <row r="369" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A369" s="32" t="s">
         <v>139</v>
       </c>
@@ -23702,7 +23696,7 @@
       <c r="AC369" s="31"/>
       <c r="AD369" s="31"/>
     </row>
-    <row r="370" spans="1:30">
+    <row r="370" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A370" s="32" t="s">
         <v>142</v>
       </c>
@@ -23764,7 +23758,7 @@
       <c r="AC370" s="31"/>
       <c r="AD370" s="31"/>
     </row>
-    <row r="371" spans="1:30">
+    <row r="371" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A371" s="32" t="s">
         <v>144</v>
       </c>
@@ -23830,7 +23824,7 @@
       <c r="AC371" s="31"/>
       <c r="AD371" s="31"/>
     </row>
-    <row r="372" spans="1:30">
+    <row r="372" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A372" s="32"/>
       <c r="B372" s="32"/>
       <c r="C372" s="32"/>
@@ -23874,7 +23868,7 @@
       <c r="AC372" s="31"/>
       <c r="AD372" s="31"/>
     </row>
-    <row r="373" spans="1:30">
+    <row r="373" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A373" s="32"/>
       <c r="B373" s="32"/>
       <c r="C373" s="32"/>
@@ -23916,7 +23910,7 @@
       <c r="AC373" s="31"/>
       <c r="AD373" s="31"/>
     </row>
-    <row r="374" spans="1:30">
+    <row r="374" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A374" s="32" t="s">
         <v>133</v>
       </c>
@@ -23973,7 +23967,7 @@
       <c r="AC374" s="31"/>
       <c r="AD374" s="31"/>
     </row>
-    <row r="375" spans="1:30" ht="15">
+    <row r="375" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A375" s="31"/>
       <c r="B375" s="31"/>
       <c r="C375" s="31"/>
@@ -24017,7 +24011,7 @@
       <c r="AC375" s="31"/>
       <c r="AD375" s="31"/>
     </row>
-    <row r="376" spans="1:30">
+    <row r="376" spans="1:30" x14ac:dyDescent="0.2">
       <c r="L376" s="41" t="s">
         <v>902</v>
       </c>
@@ -24037,7 +24031,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="377" spans="1:30" ht="15">
+    <row r="377" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A377" s="31"/>
       <c r="B377" s="31"/>
       <c r="C377" s="31"/>
@@ -24079,7 +24073,7 @@
       <c r="AC377" s="31"/>
       <c r="AD377" s="31"/>
     </row>
-    <row r="378" spans="1:30">
+    <row r="378" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A378" s="31"/>
       <c r="B378" s="31"/>
       <c r="C378" s="31"/>
@@ -24123,7 +24117,7 @@
       <c r="AC378" s="31"/>
       <c r="AD378" s="31"/>
     </row>
-    <row r="379" spans="1:30">
+    <row r="379" spans="1:30" x14ac:dyDescent="0.2">
       <c r="I379" s="37" t="s">
         <v>908</v>
       </c>
@@ -24137,7 +24131,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="380" spans="1:30">
+    <row r="380" spans="1:30" x14ac:dyDescent="0.2">
       <c r="I380" s="39" t="s">
         <v>909</v>
       </c>
@@ -24163,6 +24157,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008ECAB31773B3D64A955B79DCECF3D75D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2078a7c437835ce6ccc54ed572140080">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1812b7d3-e7a1-454a-96a7-d89f9c45d61a" xmlns:ns3="6a4f18d6-d02c-47de-8192-877c1ae6ba95" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5cdadb961a881ff75adc1ded15049d8" ns2:_="" ns3:_="">
     <xsd:import namespace="1812b7d3-e7a1-454a-96a7-d89f9c45d61a"/>
@@ -24371,29 +24380,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7B56D4F-9D08-45D2-996A-61D240C39ECD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A34CCDD6-A4F8-4456-9C15-5089C1925358}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F84129F-A8D5-4CF9-883A-6E8C05FEA359}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F84129F-A8D5-4CF9-883A-6E8C05FEA359}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A34CCDD6-A4F8-4456-9C15-5089C1925358}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7B56D4F-9D08-45D2-996A-61D240C39ECD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1812b7d3-e7a1-454a-96a7-d89f9c45d61a"/>
+    <ds:schemaRef ds:uri="6a4f18d6-d02c-47de-8192-877c1ae6ba95"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Really, really trying to fix this
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/ZoopSynth/zooper/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{E6F9FE63-518E-4809-94E4-E5D97F9282E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93273B4B-B19F-45CA-941F-D1D66B1B3128}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{E6F9FE63-518E-4809-94E4-E5D97F9282E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66F23EB9-5C5A-442D-BC8E-369D7DDB494A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchy2" sheetId="5" r:id="rId1"/>
@@ -3986,8 +3986,8 @@
   <dimension ref="A1:AH405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y200" sqref="Y200"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH140" sqref="AH140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4821,7 +4821,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="I17" s="31" t="s">
         <v>676</v>
       </c>
@@ -4861,8 +4861,11 @@
       <c r="AG17" s="30">
         <v>2018</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="AH17" s="30">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C18" s="30" t="s">
         <v>286</v>
       </c>
@@ -4915,7 +4918,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C19" s="30" t="s">
         <v>234</v>
       </c>
@@ -4963,7 +4966,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" ht="13" x14ac:dyDescent="0.3">
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
       <c r="N20" s="34"/>
@@ -4998,7 +5001,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C21" s="30" t="s">
         <v>300</v>
       </c>
@@ -5051,7 +5054,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" ht="13" x14ac:dyDescent="0.3">
       <c r="I22" s="31" t="s">
         <v>819</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
@@ -5130,7 +5133,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
@@ -5164,7 +5167,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
@@ -5207,7 +5210,7 @@
       </c>
       <c r="X25" s="50"/>
     </row>
-    <row r="26" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
@@ -5241,7 +5244,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
@@ -5278,7 +5281,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="36"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36" t="s">
@@ -5319,7 +5322,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="36"/>
       <c r="B29" s="36"/>
       <c r="C29" s="36" t="s">
@@ -5374,7 +5377,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="36"/>
       <c r="B30" s="36"/>
       <c r="C30" s="36" t="s">
@@ -5429,7 +5432,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C31" s="30" t="s">
         <v>305</v>
       </c>
@@ -5466,7 +5469,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="36"/>
       <c r="B32" s="36"/>
       <c r="C32" s="36" t="s">
@@ -5525,7 +5528,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="36"/>
       <c r="B33" s="36"/>
       <c r="C33" s="36" t="s">
@@ -5581,7 +5584,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="I34" s="31" t="s">
         <v>681</v>
       </c>
@@ -5617,7 +5620,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C35" s="30" t="s">
         <v>308</v>
       </c>
@@ -5653,7 +5656,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I36" s="31" t="s">
         <v>694</v>
       </c>
@@ -5683,7 +5686,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="I37" s="31" t="s">
         <v>692</v>
       </c>
@@ -5715,7 +5718,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C38" s="30" t="s">
         <v>267</v>
       </c>
@@ -5774,7 +5777,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D39"/>
       <c r="E39"/>
       <c r="F39"/>
@@ -5813,7 +5816,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
@@ -5845,8 +5848,14 @@
       <c r="U40" s="30" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="41" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="AG40" s="30">
+        <v>2018</v>
+      </c>
+      <c r="AH40" s="30">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
@@ -5875,7 +5884,7 @@
       <c r="W41" s="34"/>
       <c r="X41" s="34"/>
     </row>
-    <row r="42" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D42"/>
       <c r="E42"/>
       <c r="F42"/>
@@ -5901,7 +5910,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D43"/>
       <c r="E43"/>
       <c r="F43"/>
@@ -5928,7 +5937,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D44"/>
       <c r="E44"/>
       <c r="F44"/>
@@ -5960,7 +5969,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D45"/>
       <c r="E45"/>
       <c r="F45"/>
@@ -5992,7 +6001,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="I46" s="31" t="s">
         <v>976</v>
       </c>
@@ -6028,7 +6037,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="I47" s="31" t="s">
         <v>984</v>
       </c>
@@ -6064,7 +6073,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:34" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
@@ -9390,7 +9399,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B129" s="30" t="s">
         <v>81</v>
       </c>
@@ -9435,7 +9444,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="130" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="N130" s="41" t="s">
         <v>382</v>
       </c>
@@ -9471,7 +9480,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="131" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="N131" s="41" t="s">
         <v>387</v>
       </c>
@@ -9507,7 +9516,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="132" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="N132" s="41" t="s">
         <v>388</v>
       </c>
@@ -9537,7 +9546,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="133" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="N133" s="41" t="s">
         <v>391</v>
       </c>
@@ -9567,7 +9576,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="134" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A134" s="36"/>
       <c r="B134" s="36"/>
       <c r="C134" s="36"/>
@@ -9615,7 +9624,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="135" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A135" s="36"/>
       <c r="B135" s="36"/>
       <c r="C135" s="36"/>
@@ -9653,7 +9662,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="136" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A136" s="36"/>
       <c r="B136" s="36" t="s">
         <v>23</v>
@@ -9723,7 +9732,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="137" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A137" s="36"/>
       <c r="B137" s="36"/>
       <c r="C137" s="36"/>
@@ -9769,7 +9778,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="138" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A138" s="36"/>
       <c r="B138" s="36" t="s">
         <v>26</v>
@@ -9836,7 +9845,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="139" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="L139" s="39"/>
       <c r="M139" s="39"/>
       <c r="N139" s="38" t="s">
@@ -9874,7 +9883,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="140" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A140" s="36"/>
       <c r="B140" s="36"/>
       <c r="C140" s="36"/>
@@ -9928,8 +9937,11 @@
       <c r="AD140" s="30">
         <v>1995</v>
       </c>
-    </row>
-    <row r="141" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AH140" s="30">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="141" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A141" s="36"/>
       <c r="B141" s="36" t="s">
         <v>66</v>
@@ -9993,7 +10005,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="142" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A142" s="36" t="s">
         <v>105</v>
       </c>
@@ -10059,7 +10071,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:34" x14ac:dyDescent="0.25">
       <c r="L143" s="39" t="s">
         <v>22</v>
       </c>
@@ -10099,7 +10111,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="144" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A144" s="36"/>
       <c r="B144" s="36" t="s">
         <v>14</v>
@@ -20109,26 +20121,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f60d4be9-3557-4154-8f7f-0f7fc20459a7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="85a39829-3f15-4296-8687-cb7fe600cc60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F12C6E5A08C04A41BA37471DAE5B3668" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a3a391d1c404469c3015fefe5cc36b88">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="85a39829-3f15-4296-8687-cb7fe600cc60" xmlns:ns3="f60d4be9-3557-4154-8f7f-0f7fc20459a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="59dff7ddbc5431623e1e20bfe49206a8" ns2:_="" ns3:_="">
     <xsd:import namespace="85a39829-3f15-4296-8687-cb7fe600cc60"/>
@@ -20305,32 +20297,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F84129F-A8D5-4CF9-883A-6E8C05FEA359}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="85a39829-3f15-4296-8687-cb7fe600cc60"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f60d4be9-3557-4154-8f7f-0f7fc20459a7"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A34CCDD6-A4F8-4456-9C15-5089C1925358}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f60d4be9-3557-4154-8f7f-0f7fc20459a7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="85a39829-3f15-4296-8687-cb7fe600cc60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A295EE5-C46E-413A-88BC-F21FD5D85A06}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20347,4 +20334,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A34CCDD6-A4F8-4456-9C15-5089C1925358}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F84129F-A8D5-4CF9-883A-6E8C05FEA359}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="85a39829-3f15-4296-8687-cb7fe600cc60"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f60d4be9-3557-4154-8f7f-0f7fc20459a7"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fill in empty crosswalk start dates and add test to fix https://github.com/InteragencyEcologicalProgram/zooper/issues/20
</commit_message>
<xml_diff>
--- a/data-raw/crosswalk.xlsx
+++ b/data-raw/crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C3877E-CD27-47C7-BC14-01676F69DE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3DA79C-D9AC-41DB-87B5-8DDCC238F49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchy2" sheetId="5" r:id="rId1"/>
@@ -3971,9 +3971,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D2C781-127B-4418-BE4B-5645D99DF76F}">
   <dimension ref="A1:AH405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H373" sqref="H373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4627,6 +4627,9 @@
       <c r="AB10" s="29">
         <v>1972</v>
       </c>
+      <c r="AD10" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG10" s="29">
         <v>2017</v>
       </c>
@@ -5259,6 +5262,9 @@
       <c r="U24" s="29" t="s">
         <v>557</v>
       </c>
+      <c r="AD24" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG24" s="29">
         <v>2017</v>
       </c>
@@ -5916,6 +5922,9 @@
       <c r="AB37" s="29">
         <v>1972</v>
       </c>
+      <c r="AD37" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG37" s="29">
         <v>2017</v>
       </c>
@@ -6206,6 +6215,9 @@
       </c>
       <c r="AB43" s="29">
         <v>1979</v>
+      </c>
+      <c r="AD43" s="29">
+        <v>1995</v>
       </c>
       <c r="AG43" s="29">
         <v>2017</v>
@@ -7211,6 +7223,9 @@
       <c r="AB63" s="29">
         <v>1972</v>
       </c>
+      <c r="AD63" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG63" s="29">
         <v>2017</v>
       </c>
@@ -7258,6 +7273,9 @@
       </c>
       <c r="X64" s="29" t="s">
         <v>27</v>
+      </c>
+      <c r="AD64" s="29">
+        <v>2006</v>
       </c>
       <c r="AG64" s="29">
         <v>2020</v>
@@ -7770,6 +7788,9 @@
       <c r="V73" s="33"/>
       <c r="W73" s="33"/>
       <c r="X73" s="33"/>
+      <c r="AD73" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG73" s="29">
         <v>2017</v>
       </c>
@@ -8097,6 +8118,9 @@
       <c r="Z79" s="29">
         <v>1972</v>
       </c>
+      <c r="AD79" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG79" s="29">
         <v>2018</v>
       </c>
@@ -8159,6 +8183,9 @@
       </c>
       <c r="AB80" s="29">
         <v>1972</v>
+      </c>
+      <c r="AD80" s="29">
+        <v>1995</v>
       </c>
       <c r="AG80" s="29">
         <v>2017</v>
@@ -8211,6 +8238,9 @@
       <c r="X81" s="29" t="s">
         <v>31</v>
       </c>
+      <c r="AD81" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG81" s="29">
         <v>2017</v>
       </c>
@@ -8397,6 +8427,9 @@
       </c>
       <c r="AB84" s="29">
         <v>1972</v>
+      </c>
+      <c r="AD84" s="29">
+        <v>1995</v>
       </c>
       <c r="AG84" s="29">
         <v>2017</v>
@@ -16923,6 +16956,9 @@
       <c r="AB334" s="29">
         <v>2013</v>
       </c>
+      <c r="AD334" s="29">
+        <v>1995</v>
+      </c>
     </row>
     <row r="335" spans="3:33" ht="15" x14ac:dyDescent="0.25">
       <c r="D335"/>
@@ -18089,6 +18125,9 @@
       <c r="Z367" s="29">
         <v>1994</v>
       </c>
+      <c r="AB367" s="29">
+        <v>2007</v>
+      </c>
       <c r="AG367" s="29">
         <v>2017</v>
       </c>
@@ -18147,6 +18186,9 @@
       <c r="Z368" s="29">
         <v>1979</v>
       </c>
+      <c r="AB368" s="29">
+        <v>2007</v>
+      </c>
       <c r="AG368" s="29">
         <v>2017</v>
       </c>
@@ -18248,6 +18290,9 @@
       <c r="Z370" s="29">
         <v>1980</v>
       </c>
+      <c r="AB370" s="29">
+        <v>2007</v>
+      </c>
       <c r="AG370" s="29">
         <v>2017</v>
       </c>
@@ -18305,6 +18350,9 @@
       <c r="Z371" s="29">
         <v>1972</v>
       </c>
+      <c r="AB371" s="29">
+        <v>2007</v>
+      </c>
       <c r="AG371" s="29">
         <v>2017</v>
       </c>
@@ -18366,6 +18414,12 @@
       <c r="Z372" s="29">
         <v>1992</v>
       </c>
+      <c r="AB372" s="29">
+        <v>2007</v>
+      </c>
+      <c r="AD372" s="29">
+        <v>1995</v>
+      </c>
       <c r="AG372" s="29">
         <v>2017</v>
       </c>
@@ -18424,6 +18478,9 @@
       <c r="Z373" s="29">
         <v>1993</v>
       </c>
+      <c r="AB373" s="29">
+        <v>2007</v>
+      </c>
       <c r="AG373" s="29">
         <v>2017</v>
       </c>
@@ -18479,6 +18536,9 @@
       <c r="Z374" s="29">
         <v>1993</v>
       </c>
+      <c r="AB374" s="29">
+        <v>2007</v>
+      </c>
     </row>
     <row r="375" spans="1:34" x14ac:dyDescent="0.2">
       <c r="I375" s="30"/>
@@ -18546,6 +18606,12 @@
       </c>
       <c r="U376" s="30" t="s">
         <v>808</v>
+      </c>
+      <c r="Z376" s="29">
+        <v>2007</v>
+      </c>
+      <c r="AB376" s="29">
+        <v>2007</v>
       </c>
       <c r="AG376" s="29">
         <v>2017</v>

</xml_diff>